<commit_message>
zve test correction #2
Former-commit-id: d50dfccf141e9c8b35b07cc6b4799c0f067c6253
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_zve.xlsx
+++ b/tests/test_data/test_dfs_zve.xlsx
@@ -58,9 +58,6 @@
     <t>handcap_degree</t>
   </si>
   <si>
-    <t>kvbeit</t>
-  </si>
-  <si>
     <t>vorsorg</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>east</t>
+  </si>
+  <si>
+    <t>gkvbeit</t>
   </si>
 </sst>
 </file>
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,13 +483,13 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J1" t="s">
         <v>12</v>
       </c>
       <c r="K1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L1" t="s">
         <v>13</v>
@@ -501,43 +501,43 @@
         <v>4</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="P1" t="s">
         <v>3</v>
       </c>
       <c r="Q1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T1" t="s">
         <v>5</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
zve test correction #3
Former-commit-id: b06c071e1d39e89b5028ecc1a604479b1e2c8a0d
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_zve.xlsx
+++ b/tests/test_data/test_dfs_zve.xlsx
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,12 +612,12 @@
         <v>0</v>
       </c>
       <c r="W2" s="1">
-        <f>U2+MAX(E2*12-801,0)</f>
-        <v>399</v>
+        <f>U2+MAX(E2*12-801-36,0)</f>
+        <v>363</v>
       </c>
       <c r="X2" s="1">
         <f>MAX(W2-AB3,0)</f>
-        <v>399</v>
+        <v>363</v>
       </c>
       <c r="Z2">
         <f t="shared" ref="Z2:Z18" si="1">(0.6+(0.02*(T2-2005)))*((12*M2)+MIN(12*(P2+N2+0.96*O2),2800))</f>
@@ -707,12 +707,12 @@
         <v>4852.5344000000005</v>
       </c>
       <c r="W3" s="1">
-        <f t="shared" ref="W3:W25" si="6">U3+MAX(E3*12-801,0)</f>
-        <v>5251.5344000000005</v>
+        <f t="shared" ref="W3:W17" si="6">U3+MAX(E3*12-801-36,0)</f>
+        <v>5215.5344000000005</v>
       </c>
       <c r="X3" s="1">
         <f t="shared" ref="X3:X25" si="7">MAX(W3-AB4,0)</f>
-        <v>5251.5344000000005</v>
+        <v>5215.5344000000005</v>
       </c>
       <c r="Z3">
         <f t="shared" si="1"/>
@@ -803,11 +803,11 @@
       </c>
       <c r="W4" s="1">
         <f t="shared" si="6"/>
-        <v>8195.8015999999989</v>
+        <v>8159.8015999999998</v>
       </c>
       <c r="X4" s="1">
         <f t="shared" si="7"/>
-        <v>8195.8015999999989</v>
+        <v>8159.8015999999998</v>
       </c>
       <c r="Z4">
         <f t="shared" si="1"/>
@@ -898,11 +898,11 @@
       </c>
       <c r="W5" s="1">
         <f t="shared" si="6"/>
-        <v>11140.068800000001</v>
+        <v>11104.068800000001</v>
       </c>
       <c r="X5" s="1">
         <f t="shared" si="7"/>
-        <v>11140.068800000001</v>
+        <v>11104.068800000001</v>
       </c>
       <c r="Z5">
         <f t="shared" si="1"/>
@@ -993,11 +993,11 @@
       </c>
       <c r="W6" s="1">
         <f t="shared" si="6"/>
-        <v>14084.335999999999</v>
+        <v>14048.335999999999</v>
       </c>
       <c r="X6" s="1">
         <f t="shared" si="7"/>
-        <v>14084.335999999999</v>
+        <v>14048.335999999999</v>
       </c>
       <c r="Z6">
         <f t="shared" si="1"/>
@@ -1088,11 +1088,11 @@
       </c>
       <c r="W7" s="1">
         <f t="shared" si="6"/>
-        <v>51795</v>
+        <v>51759</v>
       </c>
       <c r="X7" s="1">
         <f t="shared" si="7"/>
-        <v>51795</v>
+        <v>51759</v>
       </c>
       <c r="Z7">
         <f t="shared" si="1"/>
@@ -1176,11 +1176,11 @@
       </c>
       <c r="W8" s="1">
         <f t="shared" si="6"/>
-        <v>399</v>
+        <v>363</v>
       </c>
       <c r="X8" s="1">
         <f t="shared" si="7"/>
-        <v>399</v>
+        <v>363</v>
       </c>
       <c r="Z8">
         <f t="shared" si="1"/>
@@ -1271,11 +1271,11 @@
       </c>
       <c r="W9" s="1">
         <f t="shared" si="6"/>
-        <v>5575.5280000000002</v>
+        <v>5539.5280000000002</v>
       </c>
       <c r="X9" s="1">
         <f t="shared" si="7"/>
-        <v>5575.5280000000002</v>
+        <v>5539.5280000000002</v>
       </c>
       <c r="Z9">
         <f t="shared" si="1"/>
@@ -1366,11 +1366,11 @@
       </c>
       <c r="W10" s="1">
         <f t="shared" si="6"/>
-        <v>8641.7919999999995</v>
+        <v>8605.7919999999995</v>
       </c>
       <c r="X10" s="1">
         <f t="shared" si="7"/>
-        <v>8641.7919999999995</v>
+        <v>8605.7919999999995</v>
       </c>
       <c r="Z10">
         <f t="shared" si="1"/>
@@ -1461,11 +1461,11 @@
       </c>
       <c r="W11" s="1">
         <f t="shared" si="6"/>
-        <v>11708.056</v>
+        <v>11672.056</v>
       </c>
       <c r="X11" s="1">
         <f t="shared" si="7"/>
-        <v>11708.056</v>
+        <v>11672.056</v>
       </c>
       <c r="Z11">
         <f t="shared" si="1"/>
@@ -1556,11 +1556,11 @@
       </c>
       <c r="W12" s="1">
         <f t="shared" si="6"/>
-        <v>14774.32</v>
+        <v>14738.32</v>
       </c>
       <c r="X12" s="1">
         <f t="shared" si="7"/>
-        <v>14774.32</v>
+        <v>14738.32</v>
       </c>
       <c r="Z12">
         <f t="shared" si="1"/>
@@ -1651,11 +1651,11 @@
       </c>
       <c r="W13" s="1">
         <f t="shared" si="6"/>
-        <v>47283</v>
+        <v>47247</v>
       </c>
       <c r="X13" s="1">
         <f t="shared" si="7"/>
-        <v>43779</v>
+        <v>43743</v>
       </c>
       <c r="Z13">
         <f>(0.6+(0.02*(T13-2005)))*((12*5500)+MIN(12*(P13+N13+0.96*O13),2800))</f>
@@ -1745,11 +1745,11 @@
       </c>
       <c r="W14" s="1">
         <f t="shared" si="6"/>
-        <v>17693.432000000001</v>
+        <v>17657.432000000001</v>
       </c>
       <c r="X14" s="1">
         <f t="shared" si="7"/>
-        <v>17693.432000000001</v>
+        <v>17657.432000000001</v>
       </c>
       <c r="Z14">
         <f t="shared" si="1"/>
@@ -1934,11 +1934,11 @@
       </c>
       <c r="W16" s="1">
         <f t="shared" si="6"/>
-        <v>29103</v>
+        <v>29067</v>
       </c>
       <c r="X16" s="1">
         <f t="shared" si="7"/>
-        <v>29103</v>
+        <v>29067</v>
       </c>
       <c r="Z16">
         <f t="shared" si="1"/>
@@ -2122,12 +2122,12 @@
         <v>15782.080000000002</v>
       </c>
       <c r="W18" s="1">
-        <f>U18+MAX(E18*12-1370-51,0)</f>
-        <v>29265.08</v>
+        <f>U18+MAX(E18*12-1370-51-36,0)</f>
+        <v>29229.08</v>
       </c>
       <c r="X18" s="1">
         <f t="shared" si="7"/>
-        <v>29265.08</v>
+        <v>29229.08</v>
       </c>
       <c r="Z18">
         <f t="shared" si="1"/>
@@ -2310,7 +2310,7 @@
         <v>13685.335999999999</v>
       </c>
       <c r="W20" s="1">
-        <f t="shared" si="6"/>
+        <f>U20+MAX(E20*12-801-36,0)</f>
         <v>13685.335999999999</v>
       </c>
       <c r="X20" s="1">
@@ -2404,7 +2404,7 @@
         <v>13685.335999999999</v>
       </c>
       <c r="W21" s="1">
-        <f t="shared" si="6"/>
+        <f>U21+MAX(E21*12-801-36,0)</f>
         <v>13685.335999999999</v>
       </c>
       <c r="X21" s="1">
@@ -2498,12 +2498,12 @@
         <v>20312.224000000002</v>
       </c>
       <c r="W22" s="1">
-        <f>U22+MAX(E22*12-(2*801),0)</f>
-        <v>24824.224000000002</v>
+        <f>U22+MAX(E22*12-(2*801)-(2*36),0)</f>
+        <v>24752.224000000002</v>
       </c>
       <c r="X22" s="1">
         <f t="shared" si="7"/>
-        <v>21110.224000000002</v>
+        <v>21038.224000000002</v>
       </c>
       <c r="Z22">
         <f t="shared" si="16"/>
@@ -2593,12 +2593,12 @@
         <v>20312.224000000002</v>
       </c>
       <c r="W23" s="1">
-        <f>U23+MAX(E22*12-(2*801),0)</f>
-        <v>24824.224000000002</v>
+        <f>U23+MAX(E22*12-(2*801)-(2*36),0)</f>
+        <v>24752.224000000002</v>
       </c>
       <c r="X23" s="1">
         <f t="shared" si="7"/>
-        <v>24824.224000000002</v>
+        <v>24752.224000000002</v>
       </c>
       <c r="Z23">
         <f t="shared" si="16"/>
@@ -2687,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="W24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="W3:W25" si="22">U24+MAX(E24*12-801,0)</f>
         <v>0</v>
       </c>
       <c r="X24" s="1">
@@ -2780,7 +2780,7 @@
         <v>0</v>
       </c>
       <c r="W25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="X25" s="1">

</xml_diff>

<commit_message>
zve test correction #4
Former-commit-id: cc26a2d095fcde8f1e1c5f639d80e7f0e043c728
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_zve.xlsx
+++ b/tests/test_data/test_dfs_zve.xlsx
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,11 +620,11 @@
         <v>363</v>
       </c>
       <c r="Z2">
-        <f t="shared" ref="Z2:Z18" si="1">(0.6+(0.02*(T2-2005)))*((12*M2)+MIN(12*(P2+N2+0.96*O2),2800))</f>
+        <f>((0.6+(0.02*(T2-2005)))*(12*M2))+MIN(12*(P2+N2+0.96*O2),2800)</f>
         <v>0</v>
       </c>
       <c r="AA2">
-        <f t="shared" ref="AA2:AA7" si="2">(12*D2+(12*C2 - 1000)*(C2&gt;450))</f>
+        <f t="shared" ref="AA2:AA7" si="1">(12*D2+(12*C2 - 1000)*(C2&gt;450))</f>
         <v>0</v>
       </c>
       <c r="AB2">
@@ -633,7 +633,7 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A13" si="3">B3</f>
+        <f t="shared" ref="A3:A13" si="2">B3</f>
         <v>2</v>
       </c>
       <c r="B3">
@@ -699,27 +699,27 @@
         <v>2018</v>
       </c>
       <c r="U3" s="2">
-        <f t="shared" ref="U3:U13" si="4">MAX(AA3-Z3-36,0)</f>
-        <v>4852.5344000000005</v>
+        <f t="shared" ref="U3:U13" si="3">MAX(AA3-Z3-36,0)</f>
+        <v>4739.84</v>
       </c>
       <c r="V3" s="2">
-        <f t="shared" ref="V3:V25" si="5">U3-AB3</f>
-        <v>4852.5344000000005</v>
+        <f t="shared" ref="V3:V25" si="4">U3-AB3</f>
+        <v>4739.84</v>
       </c>
       <c r="W3" s="1">
-        <f t="shared" ref="W3:W17" si="6">U3+MAX(E3*12-801-36,0)</f>
-        <v>5215.5344000000005</v>
+        <f t="shared" ref="W3:W17" si="5">U3+MAX(E3*12-801-36,0)</f>
+        <v>5102.84</v>
       </c>
       <c r="X3" s="1">
-        <f t="shared" ref="X3:X25" si="7">MAX(W3-AB4,0)</f>
-        <v>5215.5344000000005</v>
+        <f t="shared" ref="X3:X25" si="6">MAX(W3-AB4,0)</f>
+        <v>5102.84</v>
       </c>
       <c r="Z3">
+        <f t="shared" ref="Z3:Z25" si="7">((0.6+(0.02*(T3-2005)))*(12*M3))+MIN(12*(P3+N3+0.96*O3),2800)</f>
+        <v>1424.16</v>
+      </c>
+      <c r="AA3">
         <f t="shared" si="1"/>
-        <v>1311.4656</v>
-      </c>
-      <c r="AA3">
-        <f t="shared" si="2"/>
         <v>6200</v>
       </c>
       <c r="AB3">
@@ -728,7 +728,7 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="B4">
@@ -794,27 +794,27 @@
         <v>2018</v>
       </c>
       <c r="U4" s="2">
+        <f t="shared" si="3"/>
+        <v>7627.76</v>
+      </c>
+      <c r="V4" s="2">
         <f t="shared" si="4"/>
-        <v>7796.8015999999998</v>
-      </c>
-      <c r="V4" s="2">
+        <v>7627.76</v>
+      </c>
+      <c r="W4" s="1">
         <f t="shared" si="5"/>
-        <v>7796.8015999999998</v>
-      </c>
-      <c r="W4" s="1">
+        <v>7990.76</v>
+      </c>
+      <c r="X4" s="1">
         <f t="shared" si="6"/>
-        <v>8159.8015999999998</v>
-      </c>
-      <c r="X4" s="1">
+        <v>7990.76</v>
+      </c>
+      <c r="Z4">
         <f t="shared" si="7"/>
-        <v>8159.8015999999998</v>
-      </c>
-      <c r="Z4">
+        <v>2136.2399999999998</v>
+      </c>
+      <c r="AA4">
         <f t="shared" si="1"/>
-        <v>1967.1984</v>
-      </c>
-      <c r="AA4">
-        <f t="shared" si="2"/>
         <v>9800</v>
       </c>
       <c r="AB4">
@@ -823,7 +823,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B5">
@@ -889,27 +889,27 @@
         <v>2018</v>
       </c>
       <c r="U5" s="2">
+        <f t="shared" si="3"/>
+        <v>10515.68</v>
+      </c>
+      <c r="V5" s="2">
         <f t="shared" si="4"/>
-        <v>10741.068800000001</v>
-      </c>
-      <c r="V5" s="2">
+        <v>10515.68</v>
+      </c>
+      <c r="W5" s="1">
         <f t="shared" si="5"/>
-        <v>10741.068800000001</v>
-      </c>
-      <c r="W5" s="1">
+        <v>10878.68</v>
+      </c>
+      <c r="X5" s="1">
         <f t="shared" si="6"/>
-        <v>11104.068800000001</v>
-      </c>
-      <c r="X5" s="1">
+        <v>10878.68</v>
+      </c>
+      <c r="Z5">
         <f t="shared" si="7"/>
-        <v>11104.068800000001</v>
-      </c>
-      <c r="Z5">
+        <v>2848.32</v>
+      </c>
+      <c r="AA5">
         <f t="shared" si="1"/>
-        <v>2622.9312</v>
-      </c>
-      <c r="AA5">
-        <f t="shared" si="2"/>
         <v>13400</v>
       </c>
       <c r="AB5">
@@ -918,7 +918,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B6">
@@ -984,27 +984,27 @@
         <v>2018</v>
       </c>
       <c r="U6" s="2">
+        <f t="shared" si="3"/>
+        <v>13403.6</v>
+      </c>
+      <c r="V6" s="2">
         <f t="shared" si="4"/>
-        <v>13685.335999999999</v>
-      </c>
-      <c r="V6" s="2">
+        <v>13403.6</v>
+      </c>
+      <c r="W6" s="1">
         <f t="shared" si="5"/>
-        <v>13685.335999999999</v>
-      </c>
-      <c r="W6" s="1">
+        <v>13766.6</v>
+      </c>
+      <c r="X6" s="1">
         <f t="shared" si="6"/>
-        <v>14048.335999999999</v>
-      </c>
-      <c r="X6" s="1">
+        <v>13766.6</v>
+      </c>
+      <c r="Z6">
         <f t="shared" si="7"/>
-        <v>14048.335999999999</v>
-      </c>
-      <c r="Z6">
+        <v>3560.3999999999996</v>
+      </c>
+      <c r="AA6">
         <f t="shared" si="1"/>
-        <v>3278.6639999999998</v>
-      </c>
-      <c r="AA6">
-        <f t="shared" si="2"/>
         <v>17000</v>
       </c>
       <c r="AB6">
@@ -1013,7 +1013,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B7">
@@ -1079,27 +1079,27 @@
         <v>2018</v>
       </c>
       <c r="U7" s="2">
+        <f t="shared" si="3"/>
+        <v>51004</v>
+      </c>
+      <c r="V7" s="2">
         <f t="shared" si="4"/>
-        <v>51396</v>
-      </c>
-      <c r="V7" s="2">
+        <v>51004</v>
+      </c>
+      <c r="W7" s="1">
         <f t="shared" si="5"/>
-        <v>51396</v>
-      </c>
-      <c r="W7" s="1">
+        <v>51367</v>
+      </c>
+      <c r="X7" s="1">
         <f t="shared" si="6"/>
-        <v>51759</v>
-      </c>
-      <c r="X7" s="1">
+        <v>51367</v>
+      </c>
+      <c r="Z7">
         <f t="shared" si="7"/>
-        <v>51759</v>
-      </c>
-      <c r="Z7">
+        <v>7960</v>
+      </c>
+      <c r="AA7">
         <f t="shared" si="1"/>
-        <v>7568</v>
-      </c>
-      <c r="AA7">
-        <f t="shared" si="2"/>
         <v>59000</v>
       </c>
       <c r="AB7">
@@ -1108,7 +1108,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B8">
@@ -1167,23 +1167,23 @@
         <v>2010</v>
       </c>
       <c r="U8" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V8" s="2">
+      <c r="W8" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W8" s="1">
+        <v>363</v>
+      </c>
+      <c r="X8" s="1">
         <f t="shared" si="6"/>
         <v>363</v>
       </c>
-      <c r="X8" s="1">
+      <c r="Z8">
         <f t="shared" si="7"/>
-        <v>363</v>
-      </c>
-      <c r="Z8">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA8">
@@ -1196,7 +1196,7 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B9">
@@ -1262,24 +1262,24 @@
         <v>2010</v>
       </c>
       <c r="U9" s="2">
+        <f t="shared" si="3"/>
+        <v>4935.04</v>
+      </c>
+      <c r="V9" s="2">
         <f t="shared" si="4"/>
-        <v>5176.5280000000002</v>
-      </c>
-      <c r="V9" s="2">
+        <v>4935.04</v>
+      </c>
+      <c r="W9" s="1">
         <f t="shared" si="5"/>
-        <v>5176.5280000000002</v>
-      </c>
-      <c r="W9" s="1">
+        <v>5298.04</v>
+      </c>
+      <c r="X9" s="1">
         <f t="shared" si="6"/>
-        <v>5539.5280000000002</v>
-      </c>
-      <c r="X9" s="1">
+        <v>5298.04</v>
+      </c>
+      <c r="Z9">
         <f t="shared" si="7"/>
-        <v>5539.5280000000002</v>
-      </c>
-      <c r="Z9">
-        <f t="shared" si="1"/>
-        <v>1067.472</v>
+        <v>1308.96</v>
       </c>
       <c r="AA9">
         <f t="shared" si="9"/>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="B10">
@@ -1357,24 +1357,24 @@
         <v>2010</v>
       </c>
       <c r="U10" s="2">
+        <f t="shared" si="3"/>
+        <v>7880.5599999999995</v>
+      </c>
+      <c r="V10" s="2">
         <f t="shared" si="4"/>
-        <v>8242.7919999999995</v>
-      </c>
-      <c r="V10" s="2">
+        <v>7880.5599999999995</v>
+      </c>
+      <c r="W10" s="1">
         <f t="shared" si="5"/>
-        <v>8242.7919999999995</v>
-      </c>
-      <c r="W10" s="1">
+        <v>8243.56</v>
+      </c>
+      <c r="X10" s="1">
         <f t="shared" si="6"/>
-        <v>8605.7919999999995</v>
-      </c>
-      <c r="X10" s="1">
+        <v>8243.56</v>
+      </c>
+      <c r="Z10">
         <f t="shared" si="7"/>
-        <v>8605.7919999999995</v>
-      </c>
-      <c r="Z10">
-        <f t="shared" si="1"/>
-        <v>1601.2079999999999</v>
+        <v>1963.44</v>
       </c>
       <c r="AA10">
         <f t="shared" si="9"/>
@@ -1386,7 +1386,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="B11">
@@ -1452,24 +1452,24 @@
         <v>2010</v>
       </c>
       <c r="U11" s="2">
+        <f t="shared" si="3"/>
+        <v>10826.08</v>
+      </c>
+      <c r="V11" s="2">
         <f t="shared" si="4"/>
-        <v>11309.056</v>
-      </c>
-      <c r="V11" s="2">
+        <v>10826.08</v>
+      </c>
+      <c r="W11" s="1">
         <f t="shared" si="5"/>
-        <v>11309.056</v>
-      </c>
-      <c r="W11" s="1">
+        <v>11189.08</v>
+      </c>
+      <c r="X11" s="1">
         <f t="shared" si="6"/>
-        <v>11672.056</v>
-      </c>
-      <c r="X11" s="1">
+        <v>11189.08</v>
+      </c>
+      <c r="Z11">
         <f t="shared" si="7"/>
-        <v>11672.056</v>
-      </c>
-      <c r="Z11">
-        <f t="shared" si="1"/>
-        <v>2134.944</v>
+        <v>2617.92</v>
       </c>
       <c r="AA11">
         <f t="shared" si="9"/>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="B12">
@@ -1547,24 +1547,24 @@
         <v>2010</v>
       </c>
       <c r="U12" s="2">
+        <f t="shared" si="3"/>
+        <v>13771.6</v>
+      </c>
+      <c r="V12" s="2">
         <f t="shared" si="4"/>
-        <v>14375.32</v>
-      </c>
-      <c r="V12" s="2">
+        <v>13771.6</v>
+      </c>
+      <c r="W12" s="1">
         <f t="shared" si="5"/>
-        <v>14375.32</v>
-      </c>
-      <c r="W12" s="1">
+        <v>14134.6</v>
+      </c>
+      <c r="X12" s="1">
         <f t="shared" si="6"/>
-        <v>14738.32</v>
-      </c>
-      <c r="X12" s="1">
+        <v>14134.6</v>
+      </c>
+      <c r="Z12">
         <f t="shared" si="7"/>
-        <v>14738.32</v>
-      </c>
-      <c r="Z12">
-        <f t="shared" si="1"/>
-        <v>2668.6799999999994</v>
+        <v>3272.3999999999996</v>
       </c>
       <c r="AA12">
         <f t="shared" si="9"/>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="B13">
@@ -1642,24 +1642,24 @@
         <v>2010</v>
       </c>
       <c r="U13" s="2">
+        <f t="shared" si="3"/>
+        <v>85524</v>
+      </c>
+      <c r="V13" s="2">
         <f t="shared" si="4"/>
-        <v>46884</v>
-      </c>
-      <c r="V13" s="2">
+        <v>85524</v>
+      </c>
+      <c r="W13" s="1">
         <f t="shared" si="5"/>
-        <v>46884</v>
-      </c>
-      <c r="W13" s="1">
+        <v>85887</v>
+      </c>
+      <c r="X13" s="1">
         <f t="shared" si="6"/>
-        <v>47247</v>
-      </c>
-      <c r="X13" s="1">
+        <v>82383</v>
+      </c>
+      <c r="Z13">
         <f t="shared" si="7"/>
-        <v>43743</v>
-      </c>
-      <c r="Z13">
-        <f>(0.6+(0.02*(T13-2005)))*((12*5500)+MIN(12*(P13+N13+0.96*O13),2800))</f>
-        <v>48160</v>
+        <v>9520</v>
       </c>
       <c r="AA13">
         <f t="shared" si="9"/>
@@ -1737,23 +1737,23 @@
       </c>
       <c r="U14" s="2">
         <f>MAX(AA14-Z14-36-1908,0)</f>
-        <v>17294.432000000001</v>
+        <v>16596.8</v>
       </c>
       <c r="V14" s="2">
+        <f t="shared" si="4"/>
+        <v>13092.8</v>
+      </c>
+      <c r="W14" s="1">
         <f t="shared" si="5"/>
-        <v>13790.432000000001</v>
-      </c>
-      <c r="W14" s="1">
+        <v>16959.8</v>
+      </c>
+      <c r="X14" s="1">
         <f t="shared" si="6"/>
-        <v>17657.432000000001</v>
-      </c>
-      <c r="X14" s="1">
+        <v>16959.8</v>
+      </c>
+      <c r="Z14">
         <f t="shared" si="7"/>
-        <v>17657.432000000001</v>
-      </c>
-      <c r="Z14">
-        <f t="shared" si="1"/>
-        <v>3761.5679999999998</v>
+        <v>4459.2</v>
       </c>
       <c r="AA14">
         <f>(12*D14+(12*C14 - 1000)*(C14&gt;450))</f>
@@ -1835,19 +1835,19 @@
         <v>0</v>
       </c>
       <c r="V15" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W15" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W15" s="1">
+      <c r="X15" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X15" s="1">
+      <c r="Z15">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z15">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA15">
@@ -1926,23 +1926,23 @@
       </c>
       <c r="U16" s="2">
         <f>MAX(AA16-Z16-36-1908,0)</f>
-        <v>28704</v>
+        <v>27808</v>
       </c>
       <c r="V16" s="2">
+        <f t="shared" si="4"/>
+        <v>24796</v>
+      </c>
+      <c r="W16" s="1">
         <f t="shared" si="5"/>
-        <v>25692</v>
-      </c>
-      <c r="W16" s="1">
+        <v>28171</v>
+      </c>
+      <c r="X16" s="1">
         <f t="shared" si="6"/>
-        <v>29067</v>
-      </c>
-      <c r="X16" s="1">
+        <v>28171</v>
+      </c>
+      <c r="Z16">
         <f t="shared" si="7"/>
-        <v>29067</v>
-      </c>
-      <c r="Z16">
-        <f t="shared" si="1"/>
-        <v>4352</v>
+        <v>5248</v>
       </c>
       <c r="AA16">
         <f>(12*D16+(12*C16 - 1000)*(C16&gt;450))</f>
@@ -2024,19 +2024,19 @@
         <v>0</v>
       </c>
       <c r="V17" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W17" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W17" s="1">
+      <c r="X17" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X17" s="1">
+      <c r="Z17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z17">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA17">
@@ -2115,23 +2115,23 @@
       </c>
       <c r="U18" s="2">
         <f>MAX(AA18-Z18-36-1308,0)</f>
-        <v>18686.080000000002</v>
+        <v>17612.8</v>
       </c>
       <c r="V18" s="2">
-        <f t="shared" si="5"/>
-        <v>15782.080000000002</v>
+        <f t="shared" si="4"/>
+        <v>14708.8</v>
       </c>
       <c r="W18" s="1">
         <f>U18+MAX(E18*12-1370-51-36,0)</f>
-        <v>29229.08</v>
+        <v>28155.8</v>
       </c>
       <c r="X18" s="1">
+        <f t="shared" si="6"/>
+        <v>28155.8</v>
+      </c>
+      <c r="Z18">
         <f t="shared" si="7"/>
-        <v>29229.08</v>
-      </c>
-      <c r="Z18">
-        <f t="shared" si="1"/>
-        <v>3049.9199999999996</v>
+        <v>4123.2</v>
       </c>
       <c r="AA18">
         <f>(12*D18+(12*C18-920)*(C18&gt;450)+MIN((12*E18)-51-1370,0))</f>
@@ -2213,18 +2213,18 @@
         <v>0</v>
       </c>
       <c r="V19" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W19" s="1">
         <v>0</v>
       </c>
       <c r="X19" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z19">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z19">
-        <f>(0.6+(0.02*(T19-2005)))*((12*M19)+MIN(12*(P19+N19+0.96*O19),2800))</f>
         <v>0</v>
       </c>
       <c r="AA19">
@@ -2303,23 +2303,23 @@
       </c>
       <c r="U20" s="2">
         <f>0.5*(AA20+AA21-(Z20+Z21)-2*36)</f>
-        <v>13685.335999999999</v>
+        <v>13403.6</v>
       </c>
       <c r="V20" s="2">
-        <f t="shared" si="5"/>
-        <v>13685.335999999999</v>
+        <f t="shared" si="4"/>
+        <v>13403.6</v>
       </c>
       <c r="W20" s="1">
         <f>U20+MAX(E20*12-801-36,0)</f>
-        <v>13685.335999999999</v>
+        <v>13403.6</v>
       </c>
       <c r="X20" s="1">
+        <f t="shared" si="6"/>
+        <v>13403.6</v>
+      </c>
+      <c r="Z20">
         <f t="shared" si="7"/>
-        <v>13685.335999999999</v>
-      </c>
-      <c r="Z20">
-        <f t="shared" ref="Z20:Z25" si="16">(0.6+(0.02*(T20-2005)))*((12*M20)+MIN(12*(P20+N20+0.96*O20),2800))</f>
-        <v>4371.5519999999997</v>
+        <v>4747.2</v>
       </c>
       <c r="AA20">
         <f t="shared" si="15"/>
@@ -2349,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <f t="shared" ref="G21:G25" si="17">T21+(65-R21)</f>
+        <f t="shared" ref="G21:G25" si="16">T21+(65-R21)</f>
         <v>2053</v>
       </c>
       <c r="H21">
@@ -2368,19 +2368,19 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" ref="M21:M25" si="18">0.1*$C21</f>
+        <f t="shared" ref="M21:M25" si="17">0.1*$C21</f>
         <v>100</v>
       </c>
       <c r="N21">
-        <f t="shared" ref="N21:N25" si="19">0.02*C21</f>
+        <f t="shared" ref="N21:N25" si="18">0.02*C21</f>
         <v>20</v>
       </c>
       <c r="O21">
-        <f t="shared" ref="O21:O25" si="20">0.08*C21</f>
+        <f t="shared" ref="O21:O25" si="19">0.08*C21</f>
         <v>80</v>
       </c>
       <c r="P21">
-        <f t="shared" ref="P21:P25" si="21">0.015*C21</f>
+        <f t="shared" ref="P21:P25" si="20">0.015*C21</f>
         <v>15</v>
       </c>
       <c r="Q21" t="b">
@@ -2397,23 +2397,23 @@
       </c>
       <c r="U21" s="2">
         <f>0.5*(AA20+AA21-(Z20+Z21)-2*36)</f>
-        <v>13685.335999999999</v>
+        <v>13403.6</v>
       </c>
       <c r="V21" s="2">
-        <f t="shared" si="5"/>
-        <v>13685.335999999999</v>
+        <f t="shared" si="4"/>
+        <v>13403.6</v>
       </c>
       <c r="W21" s="1">
         <f>U21+MAX(E21*12-801-36,0)</f>
-        <v>13685.335999999999</v>
+        <v>13403.6</v>
       </c>
       <c r="X21" s="1">
+        <f t="shared" si="6"/>
+        <v>9689.6</v>
+      </c>
+      <c r="Z21">
         <f t="shared" si="7"/>
-        <v>9971.3359999999993</v>
-      </c>
-      <c r="Z21">
-        <f t="shared" si="16"/>
-        <v>2185.7759999999998</v>
+        <v>2373.6</v>
       </c>
       <c r="AA21">
         <f t="shared" si="15"/>
@@ -2443,7 +2443,7 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2053</v>
       </c>
       <c r="H22">
@@ -2462,19 +2462,19 @@
         <v>0</v>
       </c>
       <c r="M22">
+        <f t="shared" si="17"/>
+        <v>300</v>
+      </c>
+      <c r="N22">
         <f t="shared" si="18"/>
-        <v>300</v>
-      </c>
-      <c r="N22">
+        <v>60</v>
+      </c>
+      <c r="O22">
         <f t="shared" si="19"/>
-        <v>60</v>
-      </c>
-      <c r="O22">
+        <v>240</v>
+      </c>
+      <c r="P22">
         <f t="shared" si="20"/>
-        <v>240</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="21"/>
         <v>45</v>
       </c>
       <c r="Q22" t="b">
@@ -2491,23 +2491,23 @@
       </c>
       <c r="U22" s="2">
         <f>0.5*(AA22+AA23-(Z22+Z23)-2*36)</f>
-        <v>24026.224000000002</v>
+        <v>23642.400000000001</v>
       </c>
       <c r="V22" s="2">
-        <f t="shared" si="5"/>
-        <v>20312.224000000002</v>
+        <f t="shared" si="4"/>
+        <v>19928.400000000001</v>
       </c>
       <c r="W22" s="1">
         <f>U22+MAX(E22*12-(2*801)-(2*36),0)</f>
-        <v>24752.224000000002</v>
+        <v>24368.400000000001</v>
       </c>
       <c r="X22" s="1">
+        <f t="shared" si="6"/>
+        <v>20654.400000000001</v>
+      </c>
+      <c r="Z22">
         <f t="shared" si="7"/>
-        <v>21038.224000000002</v>
-      </c>
-      <c r="Z22">
-        <f t="shared" si="16"/>
-        <v>5504</v>
+        <v>5896</v>
       </c>
       <c r="AA22">
         <f t="shared" si="15"/>
@@ -2538,7 +2538,7 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2053</v>
       </c>
       <c r="H23">
@@ -2557,19 +2557,19 @@
         <v>0</v>
       </c>
       <c r="M23">
+        <f t="shared" si="17"/>
+        <v>200</v>
+      </c>
+      <c r="N23">
         <f t="shared" si="18"/>
-        <v>200</v>
-      </c>
-      <c r="N23">
+        <v>40</v>
+      </c>
+      <c r="O23">
         <f t="shared" si="19"/>
-        <v>40</v>
-      </c>
-      <c r="O23">
+        <v>160</v>
+      </c>
+      <c r="P23">
         <f t="shared" si="20"/>
-        <v>160</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="Q23" t="b">
@@ -2586,23 +2586,23 @@
       </c>
       <c r="U23" s="2">
         <f>0.5*(AA22+AA23-(Z22+Z23)-2*36)</f>
-        <v>24026.224000000002</v>
+        <v>23642.400000000001</v>
       </c>
       <c r="V23" s="2">
-        <f t="shared" si="5"/>
-        <v>20312.224000000002</v>
+        <f t="shared" si="4"/>
+        <v>19928.400000000001</v>
       </c>
       <c r="W23" s="1">
         <f>U23+MAX(E22*12-(2*801)-(2*36),0)</f>
-        <v>24752.224000000002</v>
+        <v>24368.400000000001</v>
       </c>
       <c r="X23" s="1">
+        <f t="shared" si="6"/>
+        <v>24368.400000000001</v>
+      </c>
+      <c r="Z23">
         <f t="shared" si="7"/>
-        <v>24752.224000000002</v>
-      </c>
-      <c r="Z23">
-        <f t="shared" si="16"/>
-        <v>4371.5519999999997</v>
+        <v>4747.2</v>
       </c>
       <c r="AA23">
         <f t="shared" si="15"/>
@@ -2633,7 +2633,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2075</v>
       </c>
       <c r="H24">
@@ -2652,19 +2652,19 @@
         <v>0</v>
       </c>
       <c r="M24">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N24">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="Q24" t="b">
@@ -2683,19 +2683,19 @@
         <v>0</v>
       </c>
       <c r="V24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W24" s="1">
-        <f t="shared" ref="W3:W25" si="22">U24+MAX(E24*12-801,0)</f>
+        <f t="shared" ref="W3:W25" si="21">U24+MAX(E24*12-801,0)</f>
         <v>0</v>
       </c>
       <c r="X24" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z24">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z24">
-        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AA24">
@@ -2726,7 +2726,7 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2080</v>
       </c>
       <c r="H25">
@@ -2745,19 +2745,19 @@
         <v>0</v>
       </c>
       <c r="M25">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N25">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="Q25" t="b">
@@ -2776,19 +2776,19 @@
         <v>0</v>
       </c>
       <c r="V25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W25" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="X25" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z25">
-        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AA25">

</xml_diff>

<commit_message>
zve test correction #5
Former-commit-id: 611857343e9cfc895ba1458ec3ec6a921f988e0a
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_zve.xlsx
+++ b/tests/test_data/test_dfs_zve.xlsx
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,15 +707,15 @@
         <v>4739.84</v>
       </c>
       <c r="W3" s="1">
-        <f t="shared" ref="W3:W17" si="5">U3+MAX(E3*12-801-36,0)</f>
-        <v>5102.84</v>
+        <f>U3+MAX(E3*12-801,0)</f>
+        <v>5138.84</v>
       </c>
       <c r="X3" s="1">
-        <f t="shared" ref="X3:X25" si="6">MAX(W3-AB4,0)</f>
-        <v>5102.84</v>
+        <f t="shared" ref="X3:X25" si="5">MAX(W3-AB4,0)</f>
+        <v>5138.84</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z25" si="7">((0.6+(0.02*(T3-2005)))*(12*M3))+MIN(12*(P3+N3+0.96*O3),2800)</f>
+        <f t="shared" ref="Z3:Z25" si="6">((0.6+(0.02*(T3-2005)))*(12*M3))+MIN(12*(P3+N3+0.96*O3),2800)</f>
         <v>1424.16</v>
       </c>
       <c r="AA3">
@@ -766,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M13" si="8">0.1*C4</f>
+        <f t="shared" ref="M4:M13" si="7">0.1*C4</f>
         <v>90</v>
       </c>
       <c r="N4">
@@ -794,7 +794,7 @@
         <v>2018</v>
       </c>
       <c r="U4" s="2">
-        <f t="shared" si="3"/>
+        <f>MAX(AA4-Z4-36,0)</f>
         <v>7627.76</v>
       </c>
       <c r="V4" s="2">
@@ -802,15 +802,15 @@
         <v>7627.76</v>
       </c>
       <c r="W4" s="1">
+        <f>U4+MAX(E4*12-801,0)</f>
+        <v>8026.76</v>
+      </c>
+      <c r="X4" s="1">
         <f t="shared" si="5"/>
-        <v>7990.76</v>
-      </c>
-      <c r="X4" s="1">
+        <v>8026.76</v>
+      </c>
+      <c r="Z4">
         <f t="shared" si="6"/>
-        <v>7990.76</v>
-      </c>
-      <c r="Z4">
-        <f t="shared" si="7"/>
         <v>2136.2399999999998</v>
       </c>
       <c r="AA4">
@@ -861,7 +861,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>120</v>
       </c>
       <c r="N5">
@@ -897,15 +897,15 @@
         <v>10515.68</v>
       </c>
       <c r="W5" s="1">
+        <f>U5+MAX(E5*12-801,0)</f>
+        <v>10914.68</v>
+      </c>
+      <c r="X5" s="1">
         <f t="shared" si="5"/>
-        <v>10878.68</v>
-      </c>
-      <c r="X5" s="1">
+        <v>10914.68</v>
+      </c>
+      <c r="Z5">
         <f t="shared" si="6"/>
-        <v>10878.68</v>
-      </c>
-      <c r="Z5">
-        <f t="shared" si="7"/>
         <v>2848.32</v>
       </c>
       <c r="AA5">
@@ -956,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="N6">
@@ -992,15 +992,15 @@
         <v>13403.6</v>
       </c>
       <c r="W6" s="1">
+        <f>U6+MAX(E6*12-801,0)</f>
+        <v>13802.6</v>
+      </c>
+      <c r="X6" s="1">
         <f t="shared" si="5"/>
-        <v>13766.6</v>
-      </c>
-      <c r="X6" s="1">
+        <v>13802.6</v>
+      </c>
+      <c r="Z6">
         <f t="shared" si="6"/>
-        <v>13766.6</v>
-      </c>
-      <c r="Z6">
-        <f t="shared" si="7"/>
         <v>3560.3999999999996</v>
       </c>
       <c r="AA6">
@@ -1051,7 +1051,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>500</v>
       </c>
       <c r="N7">
@@ -1087,15 +1087,15 @@
         <v>51004</v>
       </c>
       <c r="W7" s="1">
+        <f>U7+MAX(E7*12-801,0)</f>
+        <v>51403</v>
+      </c>
+      <c r="X7" s="1">
         <f t="shared" si="5"/>
-        <v>51367</v>
-      </c>
-      <c r="X7" s="1">
+        <v>51403</v>
+      </c>
+      <c r="Z7">
         <f t="shared" si="6"/>
-        <v>51367</v>
-      </c>
-      <c r="Z7">
-        <f t="shared" si="7"/>
         <v>7960</v>
       </c>
       <c r="AA7">
@@ -1175,19 +1175,19 @@
         <v>0</v>
       </c>
       <c r="W8" s="1">
+        <f>U8+MAX(E8*12-801-36,0)</f>
+        <v>363</v>
+      </c>
+      <c r="X8" s="1">
         <f t="shared" si="5"/>
         <v>363</v>
       </c>
-      <c r="X8" s="1">
+      <c r="Z8">
         <f t="shared" si="6"/>
-        <v>363</v>
-      </c>
-      <c r="Z8">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AA8">
-        <f t="shared" ref="AA8:AA13" si="9">(12*D8+(12*C8 - 920)*(C8&gt;450))</f>
+        <f t="shared" ref="AA8:AA13" si="8">(12*D8+(12*C8 - 920)*(C8&gt;450))</f>
         <v>0</v>
       </c>
       <c r="AB8">
@@ -1234,7 +1234,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="N9">
@@ -1270,19 +1270,19 @@
         <v>4935.04</v>
       </c>
       <c r="W9" s="1">
+        <f>U9+MAX(E9*12-801,0)</f>
+        <v>5334.04</v>
+      </c>
+      <c r="X9" s="1">
         <f t="shared" si="5"/>
-        <v>5298.04</v>
-      </c>
-      <c r="X9" s="1">
+        <v>5334.04</v>
+      </c>
+      <c r="Z9">
         <f t="shared" si="6"/>
-        <v>5298.04</v>
-      </c>
-      <c r="Z9">
-        <f t="shared" si="7"/>
         <v>1308.96</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>6280</v>
       </c>
       <c r="AB9">
@@ -1329,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>90</v>
       </c>
       <c r="N10">
@@ -1365,19 +1365,19 @@
         <v>7880.5599999999995</v>
       </c>
       <c r="W10" s="1">
+        <f>U10+MAX(E10*12-801,0)</f>
+        <v>8279.56</v>
+      </c>
+      <c r="X10" s="1">
         <f t="shared" si="5"/>
-        <v>8243.56</v>
-      </c>
-      <c r="X10" s="1">
+        <v>8279.56</v>
+      </c>
+      <c r="Z10">
         <f t="shared" si="6"/>
-        <v>8243.56</v>
-      </c>
-      <c r="Z10">
-        <f t="shared" si="7"/>
         <v>1963.44</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>9880</v>
       </c>
       <c r="AB10">
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>120</v>
       </c>
       <c r="N11">
@@ -1460,19 +1460,19 @@
         <v>10826.08</v>
       </c>
       <c r="W11" s="1">
+        <f>U11+MAX(E11*12-801,0)</f>
+        <v>11225.08</v>
+      </c>
+      <c r="X11" s="1">
         <f t="shared" si="5"/>
-        <v>11189.08</v>
-      </c>
-      <c r="X11" s="1">
+        <v>11225.08</v>
+      </c>
+      <c r="Z11">
         <f t="shared" si="6"/>
-        <v>11189.08</v>
-      </c>
-      <c r="Z11">
-        <f t="shared" si="7"/>
         <v>2617.92</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>13480</v>
       </c>
       <c r="AB11">
@@ -1519,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="N12">
@@ -1555,19 +1555,19 @@
         <v>13771.6</v>
       </c>
       <c r="W12" s="1">
+        <f>U12+MAX(E12*12-801,0)</f>
+        <v>14170.6</v>
+      </c>
+      <c r="X12" s="1">
         <f t="shared" si="5"/>
-        <v>14134.6</v>
-      </c>
-      <c r="X12" s="1">
+        <v>14170.6</v>
+      </c>
+      <c r="Z12">
         <f t="shared" si="6"/>
-        <v>14134.6</v>
-      </c>
-      <c r="Z12">
-        <f t="shared" si="7"/>
         <v>3272.3999999999996</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>17080</v>
       </c>
       <c r="AB12">
@@ -1614,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>800</v>
       </c>
       <c r="N13">
@@ -1650,19 +1650,19 @@
         <v>85524</v>
       </c>
       <c r="W13" s="1">
+        <f>U13+MAX(E13*12-801,0)</f>
+        <v>85923</v>
+      </c>
+      <c r="X13" s="1">
         <f t="shared" si="5"/>
-        <v>85887</v>
-      </c>
-      <c r="X13" s="1">
+        <v>82419</v>
+      </c>
+      <c r="Z13">
         <f t="shared" si="6"/>
-        <v>82383</v>
-      </c>
-      <c r="Z13">
-        <f t="shared" si="7"/>
         <v>9520</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>95080</v>
       </c>
       <c r="AB13">
@@ -1712,15 +1712,15 @@
         <v>200</v>
       </c>
       <c r="N14">
-        <f t="shared" ref="N14:N19" si="10">0.02*C14</f>
+        <f t="shared" ref="N14:N19" si="9">0.02*C14</f>
         <v>40</v>
       </c>
       <c r="O14">
-        <f t="shared" ref="O14:O19" si="11">0.08*C14</f>
+        <f t="shared" ref="O14:O19" si="10">0.08*C14</f>
         <v>160</v>
       </c>
       <c r="P14">
-        <f t="shared" ref="P14:P19" si="12">0.015*C14</f>
+        <f t="shared" ref="P14:P19" si="11">0.015*C14</f>
         <v>30</v>
       </c>
       <c r="Q14" t="b">
@@ -1744,15 +1744,15 @@
         <v>13092.8</v>
       </c>
       <c r="W14" s="1">
+        <f>U14+MAX(E14*12-801,0)</f>
+        <v>16995.8</v>
+      </c>
+      <c r="X14" s="1">
         <f t="shared" si="5"/>
-        <v>16959.8</v>
-      </c>
-      <c r="X14" s="1">
+        <v>16995.8</v>
+      </c>
+      <c r="Z14">
         <f t="shared" si="6"/>
-        <v>16959.8</v>
-      </c>
-      <c r="Z14">
-        <f t="shared" si="7"/>
         <v>4459.2</v>
       </c>
       <c r="AA14">
@@ -1807,15 +1807,15 @@
         <v>0</v>
       </c>
       <c r="N15">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q15" t="b">
@@ -1831,7 +1831,7 @@
         <v>2012</v>
       </c>
       <c r="U15" s="2">
-        <f t="shared" ref="U15:U19" si="13">MAX(AA15-Z15-36,0)</f>
+        <f t="shared" ref="U15:U19" si="12">MAX(AA15-Z15-36,0)</f>
         <v>0</v>
       </c>
       <c r="V15" s="2">
@@ -1839,15 +1839,15 @@
         <v>0</v>
       </c>
       <c r="W15" s="1">
+        <f>U15+MAX(E15*12-801,0)</f>
+        <v>0</v>
+      </c>
+      <c r="X15" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="X15" s="1">
+      <c r="Z15">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Z15">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AA15">
@@ -1897,19 +1897,19 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <f t="shared" ref="M16:M19" si="14">0.1*C16</f>
+        <f t="shared" ref="M16:M19" si="13">0.1*C16</f>
         <v>300</v>
       </c>
       <c r="N16">
+        <f t="shared" si="9"/>
+        <v>60</v>
+      </c>
+      <c r="O16">
         <f t="shared" si="10"/>
-        <v>60</v>
-      </c>
-      <c r="O16">
+        <v>240</v>
+      </c>
+      <c r="P16">
         <f t="shared" si="11"/>
-        <v>240</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="12"/>
         <v>45</v>
       </c>
       <c r="Q16" t="b">
@@ -1933,15 +1933,15 @@
         <v>24796</v>
       </c>
       <c r="W16" s="1">
+        <f>U16+MAX(E16*12-801,0)</f>
+        <v>28207</v>
+      </c>
+      <c r="X16" s="1">
         <f t="shared" si="5"/>
-        <v>28171</v>
-      </c>
-      <c r="X16" s="1">
+        <v>28207</v>
+      </c>
+      <c r="Z16">
         <f t="shared" si="6"/>
-        <v>28171</v>
-      </c>
-      <c r="Z16">
-        <f t="shared" si="7"/>
         <v>5248</v>
       </c>
       <c r="AA16">
@@ -1992,19 +1992,19 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O17">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q17" t="b">
@@ -2020,7 +2020,7 @@
         <v>2009</v>
       </c>
       <c r="U17" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="V17" s="2">
@@ -2028,15 +2028,15 @@
         <v>0</v>
       </c>
       <c r="W17" s="1">
+        <f>U17+MAX(E17*12-801,0)</f>
+        <v>0</v>
+      </c>
+      <c r="X17" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="X17" s="1">
+      <c r="Z17">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Z17">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AA17">
@@ -2086,19 +2086,19 @@
         <v>0</v>
       </c>
       <c r="M18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>200</v>
       </c>
       <c r="N18">
+        <f t="shared" si="9"/>
+        <v>40</v>
+      </c>
+      <c r="O18">
         <f t="shared" si="10"/>
-        <v>40</v>
-      </c>
-      <c r="O18">
+        <v>160</v>
+      </c>
+      <c r="P18">
         <f t="shared" si="11"/>
-        <v>160</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="Q18" t="b">
@@ -2122,15 +2122,15 @@
         <v>14708.8</v>
       </c>
       <c r="W18" s="1">
-        <f>U18+MAX(E18*12-1370-51-36,0)</f>
-        <v>28155.8</v>
+        <f>U18+MAX(E18*12-1370-51,0)</f>
+        <v>28191.8</v>
       </c>
       <c r="X18" s="1">
+        <f t="shared" si="5"/>
+        <v>28191.8</v>
+      </c>
+      <c r="Z18">
         <f t="shared" si="6"/>
-        <v>28155.8</v>
-      </c>
-      <c r="Z18">
-        <f t="shared" si="7"/>
         <v>4123.2</v>
       </c>
       <c r="AA18">
@@ -2181,19 +2181,19 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O19">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q19" t="b">
@@ -2209,7 +2209,7 @@
         <v>2005</v>
       </c>
       <c r="U19" s="2">
-        <f t="shared" si="13"/>
+        <f>MAX(AA19-Z19-36,0)</f>
         <v>0</v>
       </c>
       <c r="V19" s="2">
@@ -2220,15 +2220,15 @@
         <v>0</v>
       </c>
       <c r="X19" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Z19">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Z19">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="AA19">
-        <f t="shared" ref="AA19:AA25" si="15">(12*D19+(12*C19 - 1000)*(C19&gt;450))</f>
+        <f t="shared" ref="AA19:AA25" si="14">(12*D19+(12*C19 - 1000)*(C19&gt;450))</f>
         <v>0</v>
       </c>
       <c r="AB19">
@@ -2302,27 +2302,27 @@
         <v>2018</v>
       </c>
       <c r="U20" s="2">
-        <f>0.5*(AA20+AA21-(Z20+Z21)-2*36)</f>
-        <v>13403.6</v>
+        <f t="shared" ref="U20:U21" si="15">MAX(AA20-Z20-36,0)</f>
+        <v>18216.8</v>
       </c>
       <c r="V20" s="2">
         <f t="shared" si="4"/>
-        <v>13403.6</v>
+        <v>18216.8</v>
       </c>
       <c r="W20" s="1">
-        <f>U20+MAX(E20*12-801-36,0)</f>
-        <v>13403.6</v>
+        <f>U20+MAX(E20*12-801,0)</f>
+        <v>18216.8</v>
       </c>
       <c r="X20" s="1">
+        <f t="shared" si="5"/>
+        <v>18216.8</v>
+      </c>
+      <c r="Z20">
         <f t="shared" si="6"/>
-        <v>13403.6</v>
-      </c>
-      <c r="Z20">
-        <f t="shared" si="7"/>
         <v>4747.2</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>23000</v>
       </c>
       <c r="AB20">
@@ -2396,27 +2396,27 @@
         <v>2018</v>
       </c>
       <c r="U21" s="2">
-        <f>0.5*(AA20+AA21-(Z20+Z21)-2*36)</f>
-        <v>13403.6</v>
+        <f t="shared" si="15"/>
+        <v>8590.4</v>
       </c>
       <c r="V21" s="2">
         <f t="shared" si="4"/>
-        <v>13403.6</v>
+        <v>8590.4</v>
       </c>
       <c r="W21" s="1">
-        <f>U21+MAX(E21*12-801-36,0)</f>
-        <v>13403.6</v>
+        <f>U21+MAX(E21*12-801,0)</f>
+        <v>8590.4</v>
       </c>
       <c r="X21" s="1">
+        <f t="shared" si="5"/>
+        <v>1162.3999999999996</v>
+      </c>
+      <c r="Z21">
         <f t="shared" si="6"/>
-        <v>9689.6</v>
-      </c>
-      <c r="Z21">
-        <f t="shared" si="7"/>
         <v>2373.6</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>11000</v>
       </c>
       <c r="AB21">
@@ -2491,31 +2491,31 @@
       </c>
       <c r="U22" s="2">
         <f>0.5*(AA22+AA23-(Z22+Z23)-2*36)</f>
-        <v>23642.400000000001</v>
+        <v>20784</v>
       </c>
       <c r="V22" s="2">
         <f t="shared" si="4"/>
-        <v>19928.400000000001</v>
+        <v>13356</v>
       </c>
       <c r="W22" s="1">
-        <f>U22+MAX(E22*12-(2*801)-(2*36),0)</f>
-        <v>24368.400000000001</v>
+        <f>U22+MAX(E22*12-(2*801),0)</f>
+        <v>21582</v>
       </c>
       <c r="X22" s="1">
-        <f t="shared" si="6"/>
-        <v>20654.400000000001</v>
+        <f t="shared" si="5"/>
+        <v>14154</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="7"/>
-        <v>5896</v>
+        <f>0.5*((0.6+(0.02*(T22-2005)))*(12*(M22+M23)))+MIN(12*(P22+N23+P23+N22+0.96*(O22+O23)),2*2800)</f>
+        <v>8180</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>35000</v>
       </c>
       <c r="AB22">
-        <f>7428/2</f>
-        <v>3714</v>
+        <f>7428/2*2</f>
+        <v>7428</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
@@ -2586,31 +2586,31 @@
       </c>
       <c r="U23" s="2">
         <f>0.5*(AA22+AA23-(Z22+Z23)-2*36)</f>
-        <v>23642.400000000001</v>
+        <v>20784</v>
       </c>
       <c r="V23" s="2">
         <f t="shared" si="4"/>
-        <v>19928.400000000001</v>
+        <v>13356</v>
       </c>
       <c r="W23" s="1">
-        <f>U23+MAX(E22*12-(2*801)-(2*36),0)</f>
-        <v>24368.400000000001</v>
+        <f>U23+MAX(E22*12-(2*801),0)</f>
+        <v>21582</v>
       </c>
       <c r="X23" s="1">
-        <f t="shared" si="6"/>
-        <v>24368.400000000001</v>
+        <f>MAX(W23-AB23,0)</f>
+        <v>14154</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="7"/>
-        <v>4747.2</v>
+        <f>0.5*((0.6+(0.02*(T22-2005)))*(12*(M22+M23)))+MIN(12*(P22+N23+P23+N22+0.96*(O22+O23)),2*2800)</f>
+        <v>8180</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>23000</v>
       </c>
       <c r="AB23">
-        <f>7428/2</f>
-        <v>3714</v>
+        <f>7428/2*2</f>
+        <v>7428</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
@@ -2691,15 +2691,15 @@
         <v>0</v>
       </c>
       <c r="X24" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Z24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Z24">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="AA24">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AB24">
@@ -2784,19 +2784,25 @@
         <v>0</v>
       </c>
       <c r="X25" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Z25">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Z25">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="AA25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AB25">
         <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="W27">
+        <f>2400-(2*801)</f>
+        <v>798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
zve test correction #6
Former-commit-id: bb586019d78a70d2b8d6e92eaa149455c1358800
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_zve.xlsx
+++ b/tests/test_data/test_dfs_zve.xlsx
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB27"/>
+  <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2498,12 +2498,12 @@
         <v>13356</v>
       </c>
       <c r="W22" s="1">
-        <f>U22+MAX(E22*12-(2*801),0)</f>
-        <v>21582</v>
+        <f>U22+MAX(0.5*(E22*12-(2*801)),0)</f>
+        <v>21183</v>
       </c>
       <c r="X22" s="1">
         <f t="shared" si="5"/>
-        <v>14154</v>
+        <v>13755</v>
       </c>
       <c r="Z22">
         <f>0.5*((0.6+(0.02*(T22-2005)))*(12*(M22+M23)))+MIN(12*(P22+N23+P23+N22+0.96*(O22+O23)),2*2800)</f>
@@ -2593,12 +2593,12 @@
         <v>13356</v>
       </c>
       <c r="W23" s="1">
-        <f>U23+MAX(E22*12-(2*801),0)</f>
-        <v>21582</v>
+        <f>U22+MAX(0.5*(E22*12-(2*801)),0)</f>
+        <v>21183</v>
       </c>
       <c r="X23" s="1">
         <f>MAX(W23-AB23,0)</f>
-        <v>14154</v>
+        <v>13755</v>
       </c>
       <c r="Z23">
         <f>0.5*((0.6+(0.02*(T22-2005)))*(12*(M22+M23)))+MIN(12*(P22+N23+P23+N22+0.96*(O22+O23)),2*2800)</f>
@@ -2797,12 +2797,6 @@
       </c>
       <c r="AB25">
         <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="W27">
-        <f>2400-(2*801)</f>
-        <v>798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
zve test correction #7
Former-commit-id: 637ee38024ff3aca3ef51c48eed30b4774cada19
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_zve.xlsx
+++ b/tests/test_data/test_dfs_zve.xlsx
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,11 +711,11 @@
         <v>5138.84</v>
       </c>
       <c r="X3" s="1">
-        <f t="shared" ref="X3:X25" si="5">MAX(W3-AB4,0)</f>
+        <f>MAX(W3-AB3,0)</f>
         <v>5138.84</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z25" si="6">((0.6+(0.02*(T3-2005)))*(12*M3))+MIN(12*(P3+N3+0.96*O3),2800)</f>
+        <f t="shared" ref="Z3:Z25" si="5">((0.6+(0.02*(T3-2005)))*(12*M3))+MIN(12*(P3+N3+0.96*O3),2800)</f>
         <v>1424.16</v>
       </c>
       <c r="AA3">
@@ -766,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M13" si="7">0.1*C4</f>
+        <f t="shared" ref="M4:M13" si="6">0.1*C4</f>
         <v>90</v>
       </c>
       <c r="N4">
@@ -806,11 +806,11 @@
         <v>8026.76</v>
       </c>
       <c r="X4" s="1">
+        <f t="shared" ref="X4:X25" si="7">MAX(W4-AB4,0)</f>
+        <v>8026.76</v>
+      </c>
+      <c r="Z4">
         <f t="shared" si="5"/>
-        <v>8026.76</v>
-      </c>
-      <c r="Z4">
-        <f t="shared" si="6"/>
         <v>2136.2399999999998</v>
       </c>
       <c r="AA4">
@@ -861,7 +861,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>120</v>
       </c>
       <c r="N5">
@@ -901,11 +901,11 @@
         <v>10914.68</v>
       </c>
       <c r="X5" s="1">
+        <f t="shared" si="7"/>
+        <v>10914.68</v>
+      </c>
+      <c r="Z5">
         <f t="shared" si="5"/>
-        <v>10914.68</v>
-      </c>
-      <c r="Z5">
-        <f t="shared" si="6"/>
         <v>2848.32</v>
       </c>
       <c r="AA5">
@@ -956,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="N6">
@@ -996,11 +996,11 @@
         <v>13802.6</v>
       </c>
       <c r="X6" s="1">
+        <f t="shared" si="7"/>
+        <v>13802.6</v>
+      </c>
+      <c r="Z6">
         <f t="shared" si="5"/>
-        <v>13802.6</v>
-      </c>
-      <c r="Z6">
-        <f t="shared" si="6"/>
         <v>3560.3999999999996</v>
       </c>
       <c r="AA6">
@@ -1051,7 +1051,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>500</v>
       </c>
       <c r="N7">
@@ -1091,11 +1091,11 @@
         <v>51403</v>
       </c>
       <c r="X7" s="1">
+        <f t="shared" si="7"/>
+        <v>51403</v>
+      </c>
+      <c r="Z7">
         <f t="shared" si="5"/>
-        <v>51403</v>
-      </c>
-      <c r="Z7">
-        <f t="shared" si="6"/>
         <v>7960</v>
       </c>
       <c r="AA7">
@@ -1154,6 +1154,9 @@
       <c r="O8">
         <v>0</v>
       </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
       <c r="Q8" t="b">
         <v>0</v>
       </c>
@@ -1179,11 +1182,11 @@
         <v>363</v>
       </c>
       <c r="X8" s="1">
+        <f t="shared" si="7"/>
+        <v>363</v>
+      </c>
+      <c r="Z8">
         <f t="shared" si="5"/>
-        <v>363</v>
-      </c>
-      <c r="Z8">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA8">
@@ -1234,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="N9">
@@ -1270,15 +1273,15 @@
         <v>4935.04</v>
       </c>
       <c r="W9" s="1">
-        <f>U9+MAX(E9*12-801,0)</f>
+        <f t="shared" ref="W9:W17" si="9">U9+MAX(E9*12-801,0)</f>
         <v>5334.04</v>
       </c>
       <c r="X9" s="1">
+        <f t="shared" si="7"/>
+        <v>5334.04</v>
+      </c>
+      <c r="Z9">
         <f t="shared" si="5"/>
-        <v>5334.04</v>
-      </c>
-      <c r="Z9">
-        <f t="shared" si="6"/>
         <v>1308.96</v>
       </c>
       <c r="AA9">
@@ -1329,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="N10">
@@ -1365,15 +1368,15 @@
         <v>7880.5599999999995</v>
       </c>
       <c r="W10" s="1">
-        <f>U10+MAX(E10*12-801,0)</f>
+        <f t="shared" si="9"/>
         <v>8279.56</v>
       </c>
       <c r="X10" s="1">
+        <f t="shared" si="7"/>
+        <v>8279.56</v>
+      </c>
+      <c r="Z10">
         <f t="shared" si="5"/>
-        <v>8279.56</v>
-      </c>
-      <c r="Z10">
-        <f t="shared" si="6"/>
         <v>1963.44</v>
       </c>
       <c r="AA10">
@@ -1424,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>120</v>
       </c>
       <c r="N11">
@@ -1460,15 +1463,15 @@
         <v>10826.08</v>
       </c>
       <c r="W11" s="1">
-        <f>U11+MAX(E11*12-801,0)</f>
+        <f t="shared" si="9"/>
         <v>11225.08</v>
       </c>
       <c r="X11" s="1">
+        <f t="shared" si="7"/>
+        <v>11225.08</v>
+      </c>
+      <c r="Z11">
         <f t="shared" si="5"/>
-        <v>11225.08</v>
-      </c>
-      <c r="Z11">
-        <f t="shared" si="6"/>
         <v>2617.92</v>
       </c>
       <c r="AA11">
@@ -1519,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="N12">
@@ -1555,15 +1558,15 @@
         <v>13771.6</v>
       </c>
       <c r="W12" s="1">
-        <f>U12+MAX(E12*12-801,0)</f>
+        <f t="shared" si="9"/>
         <v>14170.6</v>
       </c>
       <c r="X12" s="1">
+        <f t="shared" si="7"/>
+        <v>14170.6</v>
+      </c>
+      <c r="Z12">
         <f t="shared" si="5"/>
-        <v>14170.6</v>
-      </c>
-      <c r="Z12">
-        <f t="shared" si="6"/>
         <v>3272.3999999999996</v>
       </c>
       <c r="AA12">
@@ -1614,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>800</v>
       </c>
       <c r="N13">
@@ -1650,15 +1653,15 @@
         <v>85524</v>
       </c>
       <c r="W13" s="1">
-        <f>U13+MAX(E13*12-801,0)</f>
+        <f t="shared" si="9"/>
         <v>85923</v>
       </c>
       <c r="X13" s="1">
+        <f t="shared" si="7"/>
+        <v>85923</v>
+      </c>
+      <c r="Z13">
         <f t="shared" si="5"/>
-        <v>82419</v>
-      </c>
-      <c r="Z13">
-        <f t="shared" si="6"/>
         <v>9520</v>
       </c>
       <c r="AA13">
@@ -1712,15 +1715,15 @@
         <v>200</v>
       </c>
       <c r="N14">
-        <f t="shared" ref="N14:N19" si="9">0.02*C14</f>
+        <f t="shared" ref="N14:N19" si="10">0.02*C14</f>
         <v>40</v>
       </c>
       <c r="O14">
-        <f t="shared" ref="O14:O19" si="10">0.08*C14</f>
+        <f t="shared" ref="O14:O19" si="11">0.08*C14</f>
         <v>160</v>
       </c>
       <c r="P14">
-        <f t="shared" ref="P14:P19" si="11">0.015*C14</f>
+        <f t="shared" ref="P14:P19" si="12">0.015*C14</f>
         <v>30</v>
       </c>
       <c r="Q14" t="b">
@@ -1736,23 +1739,23 @@
         <v>2012</v>
       </c>
       <c r="U14" s="2">
-        <f>MAX(AA14-Z14-36-1908,0)</f>
-        <v>16596.8</v>
+        <f>MAX(AA14-Z14-36-1308,0)</f>
+        <v>17196.8</v>
       </c>
       <c r="V14" s="2">
         <f t="shared" si="4"/>
-        <v>13092.8</v>
+        <v>13692.8</v>
       </c>
       <c r="W14" s="1">
-        <f>U14+MAX(E14*12-801,0)</f>
-        <v>16995.8</v>
+        <f t="shared" si="9"/>
+        <v>17595.8</v>
       </c>
       <c r="X14" s="1">
+        <f t="shared" si="7"/>
+        <v>14091.8</v>
+      </c>
+      <c r="Z14">
         <f t="shared" si="5"/>
-        <v>16995.8</v>
-      </c>
-      <c r="Z14">
-        <f t="shared" si="6"/>
         <v>4459.2</v>
       </c>
       <c r="AA14">
@@ -1807,15 +1810,15 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q15" t="b">
@@ -1831,7 +1834,7 @@
         <v>2012</v>
       </c>
       <c r="U15" s="2">
-        <f t="shared" ref="U15:U19" si="12">MAX(AA15-Z15-36,0)</f>
+        <f t="shared" ref="U15:U17" si="13">MAX(AA15-Z15-36,0)</f>
         <v>0</v>
       </c>
       <c r="V15" s="2">
@@ -1839,15 +1842,15 @@
         <v>0</v>
       </c>
       <c r="W15" s="1">
-        <f>U15+MAX(E15*12-801,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X15" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z15">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Z15">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA15">
@@ -1897,19 +1900,19 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <f t="shared" ref="M16:M19" si="13">0.1*C16</f>
+        <f t="shared" ref="M16:M19" si="14">0.1*C16</f>
         <v>300</v>
       </c>
       <c r="N16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>60</v>
       </c>
       <c r="O16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>240</v>
       </c>
       <c r="P16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>45</v>
       </c>
       <c r="Q16" t="b">
@@ -1925,28 +1928,28 @@
         <v>2009</v>
       </c>
       <c r="U16" s="2">
-        <f>MAX(AA16-Z16-36-1908,0)</f>
-        <v>27808</v>
+        <f>MAX(AA16-Z16-36-1308,0)</f>
+        <v>28488</v>
       </c>
       <c r="V16" s="2">
         <f t="shared" si="4"/>
-        <v>24796</v>
+        <v>25476</v>
       </c>
       <c r="W16" s="1">
         <f>U16+MAX(E16*12-801,0)</f>
-        <v>28207</v>
+        <v>28887</v>
       </c>
       <c r="X16" s="1">
+        <f t="shared" si="7"/>
+        <v>25875</v>
+      </c>
+      <c r="Z16">
         <f t="shared" si="5"/>
-        <v>28207</v>
-      </c>
-      <c r="Z16">
-        <f t="shared" si="6"/>
         <v>5248</v>
       </c>
       <c r="AA16">
-        <f>(12*D16+(12*C16 - 1000)*(C16&gt;450))</f>
-        <v>35000</v>
+        <f>(12*D16+(12*C16 - 920)*(C16&gt;450))</f>
+        <v>35080</v>
       </c>
       <c r="AB16">
         <f>0.5*6024</f>
@@ -1992,19 +1995,19 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q17" t="b">
@@ -2020,7 +2023,7 @@
         <v>2009</v>
       </c>
       <c r="U17" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="V17" s="2">
@@ -2028,15 +2031,15 @@
         <v>0</v>
       </c>
       <c r="W17" s="1">
-        <f>U17+MAX(E17*12-801,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X17" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z17">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Z17">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA17">
@@ -2086,19 +2089,19 @@
         <v>0</v>
       </c>
       <c r="M18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>200</v>
       </c>
       <c r="N18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="O18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>160</v>
       </c>
       <c r="P18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="Q18" t="b">
@@ -2115,27 +2118,27 @@
       </c>
       <c r="U18" s="2">
         <f>MAX(AA18-Z18-36-1308,0)</f>
-        <v>17612.8</v>
+        <v>28191.8</v>
       </c>
       <c r="V18" s="2">
         <f t="shared" si="4"/>
-        <v>14708.8</v>
+        <v>25287.8</v>
       </c>
       <c r="W18" s="1">
         <f>U18+MAX(E18*12-1370-51,0)</f>
-        <v>28191.8</v>
+        <v>38770.800000000003</v>
       </c>
       <c r="X18" s="1">
+        <f t="shared" si="7"/>
+        <v>35866.800000000003</v>
+      </c>
+      <c r="Z18">
         <f t="shared" si="5"/>
-        <v>28191.8</v>
-      </c>
-      <c r="Z18">
-        <f t="shared" si="6"/>
         <v>4123.2</v>
       </c>
       <c r="AA18">
-        <f>(12*D18+(12*C18-920)*(C18&gt;450)+MIN((12*E18)-51-1370,0))</f>
-        <v>23080</v>
+        <f>(12*D18+((12*C18)-920)*(C18&gt;450)+MAX((12*E18)-51-1370,0))</f>
+        <v>33659</v>
       </c>
       <c r="AB18">
         <f>5808/2</f>
@@ -2181,19 +2184,19 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P19">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q19" t="b">
@@ -2220,15 +2223,15 @@
         <v>0</v>
       </c>
       <c r="X19" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="AA19">
-        <f t="shared" ref="AA19:AA25" si="14">(12*D19+(12*C19 - 1000)*(C19&gt;450))</f>
+        <f t="shared" ref="AA19:AA25" si="15">(12*D19+(12*C19 - 1000)*(C19&gt;450))</f>
         <v>0</v>
       </c>
       <c r="AB19">
@@ -2302,7 +2305,7 @@
         <v>2018</v>
       </c>
       <c r="U20" s="2">
-        <f t="shared" ref="U20:U21" si="15">MAX(AA20-Z20-36,0)</f>
+        <f t="shared" ref="U20:U21" si="16">MAX(AA20-Z20-36,0)</f>
         <v>18216.8</v>
       </c>
       <c r="V20" s="2">
@@ -2314,15 +2317,15 @@
         <v>18216.8</v>
       </c>
       <c r="X20" s="1">
+        <f t="shared" si="7"/>
+        <v>18216.8</v>
+      </c>
+      <c r="Z20">
         <f t="shared" si="5"/>
-        <v>18216.8</v>
-      </c>
-      <c r="Z20">
-        <f t="shared" si="6"/>
         <v>4747.2</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>23000</v>
       </c>
       <c r="AB20">
@@ -2349,7 +2352,7 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <f t="shared" ref="G21:G25" si="16">T21+(65-R21)</f>
+        <f t="shared" ref="G21:G25" si="17">T21+(65-R21)</f>
         <v>2053</v>
       </c>
       <c r="H21">
@@ -2368,19 +2371,19 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" ref="M21:M25" si="17">0.1*$C21</f>
+        <f t="shared" ref="M21:M25" si="18">0.1*$C21</f>
         <v>100</v>
       </c>
       <c r="N21">
-        <f t="shared" ref="N21:N25" si="18">0.02*C21</f>
+        <f t="shared" ref="N21:N25" si="19">0.02*C21</f>
         <v>20</v>
       </c>
       <c r="O21">
-        <f t="shared" ref="O21:O25" si="19">0.08*C21</f>
+        <f t="shared" ref="O21:O25" si="20">0.08*C21</f>
         <v>80</v>
       </c>
       <c r="P21">
-        <f t="shared" ref="P21:P25" si="20">0.015*C21</f>
+        <f t="shared" ref="P21:P25" si="21">0.015*C21</f>
         <v>15</v>
       </c>
       <c r="Q21" t="b">
@@ -2396,7 +2399,7 @@
         <v>2018</v>
       </c>
       <c r="U21" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8590.4</v>
       </c>
       <c r="V21" s="2">
@@ -2408,15 +2411,15 @@
         <v>8590.4</v>
       </c>
       <c r="X21" s="1">
+        <f t="shared" si="7"/>
+        <v>8590.4</v>
+      </c>
+      <c r="Z21">
         <f t="shared" si="5"/>
-        <v>1162.3999999999996</v>
-      </c>
-      <c r="Z21">
-        <f t="shared" si="6"/>
         <v>2373.6</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>11000</v>
       </c>
       <c r="AB21">
@@ -2443,7 +2446,7 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2053</v>
       </c>
       <c r="H22">
@@ -2462,19 +2465,19 @@
         <v>0</v>
       </c>
       <c r="M22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>300</v>
       </c>
       <c r="N22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>60</v>
       </c>
       <c r="O22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>240</v>
       </c>
       <c r="P22">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>45</v>
       </c>
       <c r="Q22" t="b">
@@ -2502,7 +2505,7 @@
         <v>21183</v>
       </c>
       <c r="X22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>13755</v>
       </c>
       <c r="Z22">
@@ -2510,7 +2513,7 @@
         <v>8180</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>35000</v>
       </c>
       <c r="AB22">
@@ -2538,7 +2541,7 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2053</v>
       </c>
       <c r="H23">
@@ -2557,19 +2560,19 @@
         <v>0</v>
       </c>
       <c r="M23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>200</v>
       </c>
       <c r="N23">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>40</v>
       </c>
       <c r="O23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>160</v>
       </c>
       <c r="P23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="Q23" t="b">
@@ -2597,7 +2600,7 @@
         <v>21183</v>
       </c>
       <c r="X23" s="1">
-        <f>MAX(W23-AB23,0)</f>
+        <f t="shared" si="7"/>
         <v>13755</v>
       </c>
       <c r="Z23">
@@ -2605,7 +2608,7 @@
         <v>8180</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>23000</v>
       </c>
       <c r="AB23">
@@ -2633,7 +2636,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2075</v>
       </c>
       <c r="H24">
@@ -2652,19 +2655,19 @@
         <v>0</v>
       </c>
       <c r="M24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="P24">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="Q24" t="b">
@@ -2687,19 +2690,19 @@
         <v>0</v>
       </c>
       <c r="W24" s="1">
-        <f t="shared" ref="W3:W25" si="21">U24+MAX(E24*12-801,0)</f>
+        <f t="shared" ref="W24:W25" si="22">U24+MAX(E24*12-801,0)</f>
         <v>0</v>
       </c>
       <c r="X24" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z24">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z24">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="AA24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB24">
@@ -2726,7 +2729,7 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2080</v>
       </c>
       <c r="H25">
@@ -2745,19 +2748,19 @@
         <v>0</v>
       </c>
       <c r="M25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="P25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="Q25" t="b">
@@ -2780,22 +2783,28 @@
         <v>0</v>
       </c>
       <c r="W25" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="X25" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z25">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z25">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="AA25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA28">
+        <f>MIN((12*E18)-51-1370,0)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
zve test correction #8
Former-commit-id: 07ad37fd248ae6f5668f34184c1ffa6a0b5b662a
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_zve.xlsx
+++ b/tests/test_data/test_dfs_zve.xlsx
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB28"/>
+  <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+      <selection activeCell="AA28" sqref="AA28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2802,12 +2802,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="AA28">
-        <f>MIN((12*E18)-51-1370,0)</f>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
zve test needs to be updated as well
Former-commit-id: 75be0b9e80465708dfb9f98be6eafc6f5bb6682b
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_zve.xlsx
+++ b/tests/test_data/test_dfs_zve.xlsx
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA28" sqref="AA28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +620,7 @@
         <v>363</v>
       </c>
       <c r="Z2">
-        <f>((0.6+(0.02*(T2-2005)))*(12*M2))+MIN(12*(P2+N2+0.96*O2),2800)</f>
+        <f>((0.6+(0.02*(T2-2005)))*(12*M2))+12*(P2+N2+0.96*O2)</f>
         <v>0</v>
       </c>
       <c r="AA2">
@@ -715,7 +715,7 @@
         <v>5138.84</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z25" si="5">((0.6+(0.02*(T3-2005)))*(12*M3))+MIN(12*(P3+N3+0.96*O3),2800)</f>
+        <f t="shared" ref="Z3:Z25" si="5">((0.6+(0.02*(T3-2005)))*(12*M3))+12*(P3+N3+0.96*O3)</f>
         <v>1424.16</v>
       </c>
       <c r="AA3">
@@ -1080,23 +1080,23 @@
       </c>
       <c r="U7" s="2">
         <f t="shared" si="3"/>
-        <v>51004</v>
+        <v>47096</v>
       </c>
       <c r="V7" s="2">
         <f t="shared" si="4"/>
-        <v>51004</v>
+        <v>47096</v>
       </c>
       <c r="W7" s="1">
         <f>U7+MAX(E7*12-801,0)</f>
-        <v>51403</v>
+        <v>47495</v>
       </c>
       <c r="X7" s="1">
         <f t="shared" si="7"/>
-        <v>51403</v>
+        <v>47495</v>
       </c>
       <c r="Z7">
         <f t="shared" si="5"/>
-        <v>7960</v>
+        <v>11868</v>
       </c>
       <c r="AA7">
         <f t="shared" si="1"/>
@@ -1646,23 +1646,23 @@
       </c>
       <c r="U13" s="2">
         <f t="shared" si="3"/>
-        <v>85524</v>
+        <v>77591.199999999997</v>
       </c>
       <c r="V13" s="2">
         <f t="shared" si="4"/>
-        <v>85524</v>
+        <v>77591.199999999997</v>
       </c>
       <c r="W13" s="1">
         <f t="shared" si="9"/>
-        <v>85923</v>
+        <v>77990.2</v>
       </c>
       <c r="X13" s="1">
         <f t="shared" si="7"/>
-        <v>85923</v>
+        <v>77990.2</v>
       </c>
       <c r="Z13">
         <f t="shared" si="5"/>
-        <v>9520</v>
+        <v>17452.8</v>
       </c>
       <c r="AA13">
         <f t="shared" si="8"/>
@@ -1929,23 +1929,23 @@
       </c>
       <c r="U16" s="2">
         <f>MAX(AA16-Z16-36-1308,0)</f>
-        <v>28488</v>
+        <v>27263.200000000001</v>
       </c>
       <c r="V16" s="2">
         <f t="shared" si="4"/>
-        <v>25476</v>
+        <v>24251.200000000001</v>
       </c>
       <c r="W16" s="1">
         <f>U16+MAX(E16*12-801,0)</f>
-        <v>28887</v>
+        <v>27662.2</v>
       </c>
       <c r="X16" s="1">
         <f t="shared" si="7"/>
-        <v>25875</v>
+        <v>24650.2</v>
       </c>
       <c r="Z16">
         <f t="shared" si="5"/>
-        <v>5248</v>
+        <v>6472.7999999999993</v>
       </c>
       <c r="AA16">
         <f>(12*D16+(12*C16 - 920)*(C16&gt;450))</f>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <v>3000</v>
@@ -2494,23 +2494,23 @@
       </c>
       <c r="U22" s="2">
         <f>0.5*(AA22+AA23-(Z22+Z23)-2*36)</f>
-        <v>20784</v>
+        <v>23030</v>
       </c>
       <c r="V22" s="2">
         <f t="shared" si="4"/>
-        <v>13356</v>
+        <v>15602</v>
       </c>
       <c r="W22" s="1">
         <f>U22+MAX(0.5*(E22*12-(2*801)),0)</f>
-        <v>21183</v>
+        <v>23429</v>
       </c>
       <c r="X22" s="1">
         <f t="shared" si="7"/>
-        <v>13755</v>
+        <v>16001</v>
       </c>
       <c r="Z22">
-        <f>0.5*((0.6+(0.02*(T22-2005)))*(12*(M22+M23)))+MIN(12*(P22+N23+P23+N22+0.96*(O22+O23)),2*2800)</f>
-        <v>8180</v>
+        <f t="shared" si="5"/>
+        <v>7120.7999999999993</v>
       </c>
       <c r="AA22">
         <f t="shared" si="15"/>
@@ -2523,10 +2523,10 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B23">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C23">
         <v>2000</v>
@@ -2589,23 +2589,23 @@
       </c>
       <c r="U23" s="2">
         <f>0.5*(AA22+AA23-(Z22+Z23)-2*36)</f>
-        <v>20784</v>
+        <v>23030</v>
       </c>
       <c r="V23" s="2">
         <f t="shared" si="4"/>
-        <v>13356</v>
+        <v>15602</v>
       </c>
       <c r="W23" s="1">
         <f>U22+MAX(0.5*(E22*12-(2*801)),0)</f>
-        <v>21183</v>
+        <v>23429</v>
       </c>
       <c r="X23" s="1">
         <f t="shared" si="7"/>
-        <v>13755</v>
+        <v>16001</v>
       </c>
       <c r="Z23">
-        <f>0.5*((0.6+(0.02*(T22-2005)))*(12*(M22+M23)))+MIN(12*(P22+N23+P23+N22+0.96*(O22+O23)),2*2800)</f>
-        <v>8180</v>
+        <f t="shared" si="5"/>
+        <v>4747.2</v>
       </c>
       <c r="AA23">
         <f t="shared" si="15"/>

</xml_diff>

<commit_message>
yet another zve test correction
Former-commit-id: 8c9371ab1d624b15927adf9d199528226fe0adf0
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_zve.xlsx
+++ b/tests/test_data/test_dfs_zve.xlsx
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +620,7 @@
         <v>363</v>
       </c>
       <c r="Z2">
-        <f>((0.6+(0.02*(T2-2005)))*(2*12*M2))-M2+12*(P2+N2+0.96*O2)</f>
+        <f>((0.6+(0.02*(T2-2005)))*(2*12*M2))-(12*M2)+12*(P2+N2+0.96*O2)</f>
         <v>0</v>
       </c>
       <c r="AA2">
@@ -700,23 +700,23 @@
       </c>
       <c r="U3" s="2">
         <f t="shared" ref="U3:U13" si="3">MAX(AA3-Z3-36,0)</f>
-        <v>4180.6399999999994</v>
+        <v>4840.6399999999994</v>
       </c>
       <c r="V3" s="2">
         <f t="shared" ref="V3:V25" si="4">U3-AB3</f>
-        <v>4180.6399999999994</v>
+        <v>4840.6399999999994</v>
       </c>
       <c r="W3" s="1">
         <f>U3+MAX(E3*12-801,0)</f>
-        <v>4579.6399999999994</v>
+        <v>5239.6399999999994</v>
       </c>
       <c r="X3" s="1">
         <f>MAX(W3-AB3,0)</f>
-        <v>4579.6399999999994</v>
+        <v>5239.6399999999994</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z25" si="5">((0.6+(0.02*(T3-2005)))*(2*12*M3))-M3+12*(P3+N3+0.96*O3)</f>
-        <v>1983.3600000000001</v>
+        <f>((0.6+(0.02*(T3-2005)))*(2*12*M3))-(12*M3)+12*(P3+N3+0.96*O3)</f>
+        <v>1323.3600000000001</v>
       </c>
       <c r="AA3">
         <f t="shared" si="1"/>
@@ -766,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M13" si="6">0.1*C4</f>
+        <f t="shared" ref="M4:M13" si="5">0.1*C4</f>
         <v>90</v>
       </c>
       <c r="N4">
@@ -795,23 +795,23 @@
       </c>
       <c r="U4" s="2">
         <f>MAX(AA4-Z4-36,0)</f>
-        <v>6788.96</v>
+        <v>7778.96</v>
       </c>
       <c r="V4" s="2">
         <f t="shared" si="4"/>
-        <v>6788.96</v>
+        <v>7778.96</v>
       </c>
       <c r="W4" s="1">
         <f>U4+MAX(E4*12-801,0)</f>
-        <v>7187.96</v>
+        <v>8177.96</v>
       </c>
       <c r="X4" s="1">
-        <f t="shared" ref="X4:X25" si="7">MAX(W4-AB4,0)</f>
-        <v>7187.96</v>
+        <f t="shared" ref="X4:X25" si="6">MAX(W4-AB4,0)</f>
+        <v>8177.96</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="5"/>
-        <v>2975.04</v>
+        <f t="shared" ref="Z4:Z25" si="7">((0.6+(0.02*(T4-2005)))*(2*12*M4))-(12*M4)+12*(P4+N4+0.96*O4)</f>
+        <v>1985.04</v>
       </c>
       <c r="AA4">
         <f t="shared" si="1"/>
@@ -861,7 +861,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>120</v>
       </c>
       <c r="N5">
@@ -890,23 +890,23 @@
       </c>
       <c r="U5" s="2">
         <f t="shared" si="3"/>
-        <v>9397.2799999999988</v>
+        <v>10717.279999999999</v>
       </c>
       <c r="V5" s="2">
         <f t="shared" si="4"/>
-        <v>9397.2799999999988</v>
+        <v>10717.279999999999</v>
       </c>
       <c r="W5" s="1">
         <f>U5+MAX(E5*12-801,0)</f>
-        <v>9796.2799999999988</v>
+        <v>11116.279999999999</v>
       </c>
       <c r="X5" s="1">
+        <f t="shared" si="6"/>
+        <v>11116.279999999999</v>
+      </c>
+      <c r="Z5">
         <f t="shared" si="7"/>
-        <v>9796.2799999999988</v>
-      </c>
-      <c r="Z5">
-        <f t="shared" si="5"/>
-        <v>3966.7200000000003</v>
+        <v>2646.7200000000003</v>
       </c>
       <c r="AA5">
         <f t="shared" si="1"/>
@@ -956,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="N6">
@@ -985,23 +985,23 @@
       </c>
       <c r="U6" s="2">
         <f t="shared" si="3"/>
-        <v>12005.6</v>
+        <v>13655.6</v>
       </c>
       <c r="V6" s="2">
         <f t="shared" si="4"/>
-        <v>12005.6</v>
+        <v>13655.6</v>
       </c>
       <c r="W6" s="1">
         <f>U6+MAX(E6*12-801,0)</f>
-        <v>12404.6</v>
+        <v>14054.6</v>
       </c>
       <c r="X6" s="1">
+        <f t="shared" si="6"/>
+        <v>14054.6</v>
+      </c>
+      <c r="Z6">
         <f t="shared" si="7"/>
-        <v>12404.6</v>
-      </c>
-      <c r="Z6">
-        <f t="shared" si="5"/>
-        <v>4958.3999999999996</v>
+        <v>3308.3999999999996</v>
       </c>
       <c r="AA6">
         <f t="shared" si="1"/>
@@ -1051,7 +1051,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>500</v>
       </c>
       <c r="N7">
@@ -1080,23 +1080,23 @@
       </c>
       <c r="U7" s="2">
         <f t="shared" si="3"/>
-        <v>42436</v>
+        <v>47936</v>
       </c>
       <c r="V7" s="2">
         <f t="shared" si="4"/>
-        <v>42436</v>
+        <v>47936</v>
       </c>
       <c r="W7" s="1">
         <f>U7+MAX(E7*12-801,0)</f>
-        <v>42835</v>
+        <v>48335</v>
       </c>
       <c r="X7" s="1">
+        <f t="shared" si="6"/>
+        <v>48335</v>
+      </c>
+      <c r="Z7">
         <f t="shared" si="7"/>
-        <v>42835</v>
-      </c>
-      <c r="Z7">
-        <f t="shared" si="5"/>
-        <v>16528</v>
+        <v>11028</v>
       </c>
       <c r="AA7">
         <f t="shared" si="1"/>
@@ -1182,11 +1182,11 @@
         <v>363</v>
       </c>
       <c r="X8" s="1">
+        <f t="shared" si="6"/>
+        <v>363</v>
+      </c>
+      <c r="Z8">
         <f t="shared" si="7"/>
-        <v>363</v>
-      </c>
-      <c r="Z8">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA8">
@@ -1237,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="N9">
@@ -1266,23 +1266,23 @@
       </c>
       <c r="U9" s="2">
         <f t="shared" si="3"/>
-        <v>4491.04</v>
+        <v>5151.04</v>
       </c>
       <c r="V9" s="2">
         <f t="shared" si="4"/>
-        <v>4491.04</v>
+        <v>5151.04</v>
       </c>
       <c r="W9" s="1">
         <f t="shared" ref="W9:W17" si="9">U9+MAX(E9*12-801,0)</f>
-        <v>4890.04</v>
+        <v>5550.04</v>
       </c>
       <c r="X9" s="1">
+        <f t="shared" si="6"/>
+        <v>5550.04</v>
+      </c>
+      <c r="Z9">
         <f t="shared" si="7"/>
-        <v>4890.04</v>
-      </c>
-      <c r="Z9">
-        <f t="shared" si="5"/>
-        <v>1752.96</v>
+        <v>1092.96</v>
       </c>
       <c r="AA9">
         <f t="shared" si="8"/>
@@ -1332,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
       <c r="N10">
@@ -1361,23 +1361,23 @@
       </c>
       <c r="U10" s="2">
         <f t="shared" si="3"/>
-        <v>7214.5599999999995</v>
+        <v>8204.56</v>
       </c>
       <c r="V10" s="2">
         <f t="shared" si="4"/>
-        <v>7214.5599999999995</v>
+        <v>8204.56</v>
       </c>
       <c r="W10" s="1">
         <f t="shared" si="9"/>
-        <v>7613.5599999999995</v>
+        <v>8603.56</v>
       </c>
       <c r="X10" s="1">
+        <f t="shared" si="6"/>
+        <v>8603.56</v>
+      </c>
+      <c r="Z10">
         <f t="shared" si="7"/>
-        <v>7613.5599999999995</v>
-      </c>
-      <c r="Z10">
-        <f t="shared" si="5"/>
-        <v>2629.44</v>
+        <v>1639.44</v>
       </c>
       <c r="AA10">
         <f t="shared" si="8"/>
@@ -1427,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>120</v>
       </c>
       <c r="N11">
@@ -1456,23 +1456,23 @@
       </c>
       <c r="U11" s="2">
         <f t="shared" si="3"/>
-        <v>9938.08</v>
+        <v>11258.08</v>
       </c>
       <c r="V11" s="2">
         <f t="shared" si="4"/>
-        <v>9938.08</v>
+        <v>11258.08</v>
       </c>
       <c r="W11" s="1">
         <f t="shared" si="9"/>
-        <v>10337.08</v>
+        <v>11657.08</v>
       </c>
       <c r="X11" s="1">
+        <f t="shared" si="6"/>
+        <v>11657.08</v>
+      </c>
+      <c r="Z11">
         <f t="shared" si="7"/>
-        <v>10337.08</v>
-      </c>
-      <c r="Z11">
-        <f t="shared" si="5"/>
-        <v>3505.92</v>
+        <v>2185.92</v>
       </c>
       <c r="AA11">
         <f t="shared" si="8"/>
@@ -1522,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="N12">
@@ -1551,23 +1551,23 @@
       </c>
       <c r="U12" s="2">
         <f t="shared" si="3"/>
-        <v>12661.6</v>
+        <v>14311.6</v>
       </c>
       <c r="V12" s="2">
         <f t="shared" si="4"/>
-        <v>12661.6</v>
+        <v>14311.6</v>
       </c>
       <c r="W12" s="1">
         <f t="shared" si="9"/>
-        <v>13060.6</v>
+        <v>14710.6</v>
       </c>
       <c r="X12" s="1">
+        <f t="shared" si="6"/>
+        <v>14710.6</v>
+      </c>
+      <c r="Z12">
         <f t="shared" si="7"/>
-        <v>13060.6</v>
-      </c>
-      <c r="Z12">
-        <f t="shared" si="5"/>
-        <v>4382.3999999999996</v>
+        <v>2732.3999999999996</v>
       </c>
       <c r="AA12">
         <f t="shared" si="8"/>
@@ -1617,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>800</v>
       </c>
       <c r="N13">
@@ -1646,23 +1646,23 @@
       </c>
       <c r="U13" s="2">
         <f t="shared" si="3"/>
-        <v>71671.199999999997</v>
+        <v>80471.199999999997</v>
       </c>
       <c r="V13" s="2">
         <f t="shared" si="4"/>
-        <v>71671.199999999997</v>
+        <v>80471.199999999997</v>
       </c>
       <c r="W13" s="1">
         <f t="shared" si="9"/>
-        <v>72070.2</v>
+        <v>80870.2</v>
       </c>
       <c r="X13" s="1">
+        <f t="shared" si="6"/>
+        <v>80870.2</v>
+      </c>
+      <c r="Z13">
         <f t="shared" si="7"/>
-        <v>72070.2</v>
-      </c>
-      <c r="Z13">
-        <f t="shared" si="5"/>
-        <v>23372.799999999999</v>
+        <v>14572.8</v>
       </c>
       <c r="AA13">
         <f t="shared" si="8"/>
@@ -1740,23 +1740,23 @@
       </c>
       <c r="U14" s="2">
         <f>MAX(AA14-Z14-36-1308,0)</f>
-        <v>15620.8</v>
+        <v>17820.8</v>
       </c>
       <c r="V14" s="2">
         <f t="shared" si="4"/>
-        <v>12116.8</v>
+        <v>14316.8</v>
       </c>
       <c r="W14" s="1">
         <f t="shared" si="9"/>
-        <v>16019.8</v>
+        <v>18219.8</v>
       </c>
       <c r="X14" s="1">
+        <f t="shared" si="6"/>
+        <v>14715.8</v>
+      </c>
+      <c r="Z14">
         <f t="shared" si="7"/>
-        <v>12515.8</v>
-      </c>
-      <c r="Z14">
-        <f t="shared" si="5"/>
-        <v>6035.2</v>
+        <v>3835.2</v>
       </c>
       <c r="AA14">
         <f>(12*D14+(12*C14 - 1000)*(C14&gt;450))</f>
@@ -1846,11 +1846,11 @@
         <v>0</v>
       </c>
       <c r="X15" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z15">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z15">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA15">
@@ -1929,23 +1929,23 @@
       </c>
       <c r="U16" s="2">
         <f>MAX(AA16-Z16-36-1308,0)</f>
-        <v>25115.200000000001</v>
+        <v>28415.200000000001</v>
       </c>
       <c r="V16" s="2">
         <f t="shared" si="4"/>
-        <v>22103.200000000001</v>
+        <v>25403.200000000001</v>
       </c>
       <c r="W16" s="1">
         <f>U16+MAX(E16*12-801,0)</f>
-        <v>25514.2</v>
+        <v>28814.2</v>
       </c>
       <c r="X16" s="1">
+        <f t="shared" si="6"/>
+        <v>25802.2</v>
+      </c>
+      <c r="Z16">
         <f t="shared" si="7"/>
-        <v>22502.2</v>
-      </c>
-      <c r="Z16">
-        <f t="shared" si="5"/>
-        <v>8620.7999999999993</v>
+        <v>5320.7999999999993</v>
       </c>
       <c r="AA16">
         <f>(12*D16+(12*C16 - 920)*(C16&gt;450))</f>
@@ -2035,11 +2035,11 @@
         <v>0</v>
       </c>
       <c r="X17" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z17">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA17">
@@ -2118,23 +2118,23 @@
       </c>
       <c r="U18" s="2">
         <f>MAX(AA18-Z18-36-1308,0)</f>
-        <v>26951.8</v>
+        <v>29151.8</v>
       </c>
       <c r="V18" s="2">
         <f t="shared" si="4"/>
-        <v>24047.8</v>
+        <v>26247.8</v>
       </c>
       <c r="W18" s="1">
         <f>U18+MAX(E18*12-1370-51,0)</f>
-        <v>37530.800000000003</v>
+        <v>39730.800000000003</v>
       </c>
       <c r="X18" s="1">
+        <f t="shared" si="6"/>
+        <v>36826.800000000003</v>
+      </c>
+      <c r="Z18">
         <f t="shared" si="7"/>
-        <v>34626.800000000003</v>
-      </c>
-      <c r="Z18">
-        <f t="shared" si="5"/>
-        <v>5363.2</v>
+        <v>3163.2</v>
       </c>
       <c r="AA18">
         <f>(12*D18+((12*C18)-920)*(C18&gt;450)+MAX((12*E18)-51-1370,0))</f>
@@ -2223,11 +2223,11 @@
         <v>0</v>
       </c>
       <c r="X19" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z19">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z19">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA19">
@@ -2306,23 +2306,23 @@
       </c>
       <c r="U20" s="2">
         <f t="shared" ref="U20:U21" si="16">MAX(AA20-Z20-36,0)</f>
-        <v>16352.8</v>
+        <v>18552.8</v>
       </c>
       <c r="V20" s="2">
         <f t="shared" si="4"/>
-        <v>16352.8</v>
+        <v>18552.8</v>
       </c>
       <c r="W20" s="1">
         <f>U20+MAX(E20*12-801,0)</f>
-        <v>16352.8</v>
+        <v>18552.8</v>
       </c>
       <c r="X20" s="1">
+        <f t="shared" si="6"/>
+        <v>18552.8</v>
+      </c>
+      <c r="Z20">
         <f t="shared" si="7"/>
-        <v>16352.8</v>
-      </c>
-      <c r="Z20">
-        <f t="shared" si="5"/>
-        <v>6611.2</v>
+        <v>4411.2</v>
       </c>
       <c r="AA20">
         <f t="shared" si="15"/>
@@ -2400,23 +2400,23 @@
       </c>
       <c r="U21" s="2">
         <f t="shared" si="16"/>
-        <v>7658.4</v>
+        <v>8758.4</v>
       </c>
       <c r="V21" s="2">
         <f t="shared" si="4"/>
-        <v>7658.4</v>
+        <v>8758.4</v>
       </c>
       <c r="W21" s="1">
         <f>U21+MAX(E21*12-801,0)</f>
-        <v>7658.4</v>
+        <v>8758.4</v>
       </c>
       <c r="X21" s="1">
+        <f t="shared" si="6"/>
+        <v>8758.4</v>
+      </c>
+      <c r="Z21">
         <f t="shared" si="7"/>
-        <v>7658.4</v>
-      </c>
-      <c r="Z21">
-        <f t="shared" si="5"/>
-        <v>3305.6</v>
+        <v>2205.6</v>
       </c>
       <c r="AA21">
         <f t="shared" si="15"/>
@@ -2494,23 +2494,23 @@
       </c>
       <c r="U22" s="2">
         <f>0.5*(AA22+AA23-(Z22+Z23)-2*36)</f>
-        <v>20700</v>
+        <v>23450</v>
       </c>
       <c r="V22" s="2">
         <f t="shared" si="4"/>
-        <v>13272</v>
+        <v>16022</v>
       </c>
       <c r="W22" s="1">
         <f>U22+MAX(0.5*(E22*12-(2*801)),0)</f>
-        <v>21099</v>
+        <v>23849</v>
       </c>
       <c r="X22" s="1">
+        <f t="shared" si="6"/>
+        <v>16421</v>
+      </c>
+      <c r="Z22">
         <f t="shared" si="7"/>
-        <v>13671</v>
-      </c>
-      <c r="Z22">
-        <f t="shared" si="5"/>
-        <v>9916.7999999999993</v>
+        <v>6616.7999999999993</v>
       </c>
       <c r="AA22">
         <f t="shared" si="15"/>
@@ -2589,23 +2589,23 @@
       </c>
       <c r="U23" s="2">
         <f>0.5*(AA22+AA23-(Z22+Z23)-2*36)</f>
-        <v>20700</v>
+        <v>23450</v>
       </c>
       <c r="V23" s="2">
         <f t="shared" si="4"/>
-        <v>13272</v>
+        <v>16022</v>
       </c>
       <c r="W23" s="1">
         <f>U22+MAX(0.5*(E22*12-(2*801)),0)</f>
-        <v>21099</v>
+        <v>23849</v>
       </c>
       <c r="X23" s="1">
+        <f t="shared" si="6"/>
+        <v>16421</v>
+      </c>
+      <c r="Z23">
         <f t="shared" si="7"/>
-        <v>13671</v>
-      </c>
-      <c r="Z23">
-        <f t="shared" si="5"/>
-        <v>6611.2</v>
+        <v>4411.2</v>
       </c>
       <c r="AA23">
         <f t="shared" si="15"/>
@@ -2694,11 +2694,11 @@
         <v>0</v>
       </c>
       <c r="X24" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z24">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z24">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA24">
@@ -2787,11 +2787,11 @@
         <v>0</v>
       </c>
       <c r="X25" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z25">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA25">

</xml_diff>

<commit_message>
yet another zve test correction	#2
Former-commit-id: 7e502d9bb14e13aa8729cb7a2095b2b3aca36f59
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_zve.xlsx
+++ b/tests/test_data/test_dfs_zve.xlsx
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:AB27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,24 +1645,24 @@
         <v>2010</v>
       </c>
       <c r="U13" s="2">
-        <f t="shared" si="3"/>
-        <v>80471.199999999997</v>
+        <f>MAX(AA13-Z13-36,0)</f>
+        <v>81684.399999999994</v>
       </c>
       <c r="V13" s="2">
         <f t="shared" si="4"/>
-        <v>80471.199999999997</v>
+        <v>81684.399999999994</v>
       </c>
       <c r="W13" s="1">
         <f t="shared" si="9"/>
-        <v>80870.2</v>
+        <v>82083.399999999994</v>
       </c>
       <c r="X13" s="1">
         <f t="shared" si="6"/>
-        <v>80870.2</v>
+        <v>82083.399999999994</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="7"/>
-        <v>14572.8</v>
+        <f>((0.6+(0.02*(T13-2005)))*(12*2*0.0995*5500))-(12*0.0995*5500)+12*(P13+N13+0.96*O13)</f>
+        <v>13359.599999999999</v>
       </c>
       <c r="AA13">
         <f t="shared" si="8"/>
@@ -2800,6 +2800,12 @@
       </c>
       <c r="AB25">
         <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z27">
+        <f>0.0995 * 5500 * 2</f>
+        <v>1094.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
yet another zve test correction	#3
Former-commit-id: 33a59bd36261baf088aac6dd15fa493015fa55c7
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_zve.xlsx
+++ b/tests/test_data/test_dfs_zve.xlsx
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB27"/>
+  <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+      <selection activeCell="Y26" sqref="Y26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,7 +699,7 @@
         <v>2018</v>
       </c>
       <c r="U3" s="2">
-        <f t="shared" ref="U3:U13" si="3">MAX(AA3-Z3-36,0)</f>
+        <f t="shared" ref="U3:U12" si="3">MAX(AA3-Z3-36,0)</f>
         <v>4840.6399999999994</v>
       </c>
       <c r="V3" s="2">
@@ -2800,12 +2800,6 @@
       </c>
       <c r="AB25">
         <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Z27">
-        <f>0.0995 * 5500 * 2</f>
-        <v>1094.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
settings reorganized. tax_transfer functions may now take 'ref' argument. bugfix in zve() function
Former-commit-id: 9e892968169b6e66c9360430c050784eeefc07c5
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_zve.xlsx
+++ b/tests/test_data/test_dfs_zve.xlsx
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y26" sqref="Y26"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +620,7 @@
         <v>363</v>
       </c>
       <c r="Z2">
-        <f>((0.6+(0.02*(T2-2005)))*(2*12*M2))-(12*M2)+12*(P2+N2+0.96*O2)</f>
+        <f>((0.6+(0.02*(T2-2005)))*(2*12*M2))-(12*M2)+MIN(12*(P2+N2+0.96*O2), 1900)</f>
         <v>0</v>
       </c>
       <c r="AA2">
@@ -715,7 +715,7 @@
         <v>5239.6399999999994</v>
       </c>
       <c r="Z3">
-        <f>((0.6+(0.02*(T3-2005)))*(2*12*M3))-(12*M3)+12*(P3+N3+0.96*O3)</f>
+        <f t="shared" ref="Z3:Z25" si="5">((0.6+(0.02*(T3-2005)))*(2*12*M3))-(12*M3)+MIN(12*(P3+N3+0.96*O3), 1900)</f>
         <v>1323.3600000000001</v>
       </c>
       <c r="AA3">
@@ -766,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M13" si="5">0.1*C4</f>
+        <f t="shared" ref="M4:M13" si="6">0.1*C4</f>
         <v>90</v>
       </c>
       <c r="N4">
@@ -806,11 +806,11 @@
         <v>8177.96</v>
       </c>
       <c r="X4" s="1">
-        <f t="shared" ref="X4:X25" si="6">MAX(W4-AB4,0)</f>
+        <f t="shared" ref="X4:X25" si="7">MAX(W4-AB4,0)</f>
         <v>8177.96</v>
       </c>
       <c r="Z4">
-        <f t="shared" ref="Z4:Z25" si="7">((0.6+(0.02*(T4-2005)))*(2*12*M4))-(12*M4)+12*(P4+N4+0.96*O4)</f>
+        <f t="shared" si="5"/>
         <v>1985.04</v>
       </c>
       <c r="AA4">
@@ -861,7 +861,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>120</v>
       </c>
       <c r="N5">
@@ -901,11 +901,11 @@
         <v>11116.279999999999</v>
       </c>
       <c r="X5" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11116.279999999999</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>2646.7200000000003</v>
       </c>
       <c r="AA5">
@@ -956,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="N6">
@@ -985,23 +985,23 @@
       </c>
       <c r="U6" s="2">
         <f t="shared" si="3"/>
-        <v>13655.6</v>
+        <v>13768</v>
       </c>
       <c r="V6" s="2">
         <f t="shared" si="4"/>
-        <v>13655.6</v>
+        <v>13768</v>
       </c>
       <c r="W6" s="1">
         <f>U6+MAX(E6*12-801,0)</f>
-        <v>14054.6</v>
+        <v>14167</v>
       </c>
       <c r="X6" s="1">
-        <f t="shared" si="6"/>
-        <v>14054.6</v>
+        <f t="shared" si="7"/>
+        <v>14167</v>
       </c>
       <c r="Z6">
-        <f t="shared" si="7"/>
-        <v>3308.3999999999996</v>
+        <f t="shared" si="5"/>
+        <v>3196</v>
       </c>
       <c r="AA6">
         <f t="shared" si="1"/>
@@ -1051,7 +1051,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>500</v>
       </c>
       <c r="N7">
@@ -1080,23 +1080,23 @@
       </c>
       <c r="U7" s="2">
         <f t="shared" si="3"/>
-        <v>47936</v>
+        <v>52744</v>
       </c>
       <c r="V7" s="2">
         <f t="shared" si="4"/>
-        <v>47936</v>
+        <v>52744</v>
       </c>
       <c r="W7" s="1">
         <f>U7+MAX(E7*12-801,0)</f>
-        <v>48335</v>
+        <v>53143</v>
       </c>
       <c r="X7" s="1">
-        <f t="shared" si="6"/>
-        <v>48335</v>
+        <f t="shared" si="7"/>
+        <v>53143</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="7"/>
-        <v>11028</v>
+        <f t="shared" si="5"/>
+        <v>6220</v>
       </c>
       <c r="AA7">
         <f t="shared" si="1"/>
@@ -1182,11 +1182,11 @@
         <v>363</v>
       </c>
       <c r="X8" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>363</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA8">
@@ -1237,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="N9">
@@ -1277,11 +1277,11 @@
         <v>5550.04</v>
       </c>
       <c r="X9" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5550.04</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1092.96</v>
       </c>
       <c r="AA9">
@@ -1332,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="N10">
@@ -1372,11 +1372,11 @@
         <v>8603.56</v>
       </c>
       <c r="X10" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8603.56</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1639.44</v>
       </c>
       <c r="AA10">
@@ -1427,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>120</v>
       </c>
       <c r="N11">
@@ -1467,11 +1467,11 @@
         <v>11657.08</v>
       </c>
       <c r="X11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11657.08</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>2185.92</v>
       </c>
       <c r="AA11">
@@ -1522,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="N12">
@@ -1551,23 +1551,23 @@
       </c>
       <c r="U12" s="2">
         <f t="shared" si="3"/>
-        <v>14311.6</v>
+        <v>14424</v>
       </c>
       <c r="V12" s="2">
         <f t="shared" si="4"/>
-        <v>14311.6</v>
+        <v>14424</v>
       </c>
       <c r="W12" s="1">
         <f t="shared" si="9"/>
-        <v>14710.6</v>
+        <v>14823</v>
       </c>
       <c r="X12" s="1">
-        <f t="shared" si="6"/>
-        <v>14710.6</v>
+        <f t="shared" si="7"/>
+        <v>14823</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="7"/>
-        <v>2732.3999999999996</v>
+        <f t="shared" si="5"/>
+        <v>2620</v>
       </c>
       <c r="AA12">
         <f t="shared" si="8"/>
@@ -1617,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>800</v>
       </c>
       <c r="N13">
@@ -1646,23 +1646,23 @@
       </c>
       <c r="U13" s="2">
         <f>MAX(AA13-Z13-36,0)</f>
-        <v>81684.399999999994</v>
+        <v>90517.2</v>
       </c>
       <c r="V13" s="2">
         <f t="shared" si="4"/>
-        <v>81684.399999999994</v>
+        <v>90517.2</v>
       </c>
       <c r="W13" s="1">
         <f t="shared" si="9"/>
-        <v>82083.399999999994</v>
+        <v>90916.2</v>
       </c>
       <c r="X13" s="1">
-        <f t="shared" si="6"/>
-        <v>82083.399999999994</v>
+        <f t="shared" si="7"/>
+        <v>90916.2</v>
       </c>
       <c r="Z13">
-        <f>((0.6+(0.02*(T13-2005)))*(12*2*0.0995*5500))-(12*0.0995*5500)+12*(P13+N13+0.96*O13)</f>
-        <v>13359.599999999999</v>
+        <f>((0.6+(0.02*(T13-2005)))*(12*2*0.0995*5500))-(12*0.0995*5500)+MIN(12*(P13+N13+0.96*O13),1900)</f>
+        <v>4526.7999999999993</v>
       </c>
       <c r="AA13">
         <f t="shared" si="8"/>
@@ -1740,23 +1740,23 @@
       </c>
       <c r="U14" s="2">
         <f>MAX(AA14-Z14-36-1308,0)</f>
-        <v>17820.8</v>
+        <v>18604</v>
       </c>
       <c r="V14" s="2">
         <f t="shared" si="4"/>
-        <v>14316.8</v>
+        <v>15100</v>
       </c>
       <c r="W14" s="1">
         <f t="shared" si="9"/>
-        <v>18219.8</v>
+        <v>19003</v>
       </c>
       <c r="X14" s="1">
-        <f t="shared" si="6"/>
-        <v>14715.8</v>
+        <f t="shared" si="7"/>
+        <v>15499</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="7"/>
-        <v>3835.2</v>
+        <f t="shared" si="5"/>
+        <v>3052</v>
       </c>
       <c r="AA14">
         <f>(12*D14+(12*C14 - 1000)*(C14&gt;450))</f>
@@ -1846,11 +1846,11 @@
         <v>0</v>
       </c>
       <c r="X15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA15">
@@ -1929,23 +1929,23 @@
       </c>
       <c r="U16" s="2">
         <f>MAX(AA16-Z16-36-1308,0)</f>
-        <v>28415.200000000001</v>
+        <v>30540</v>
       </c>
       <c r="V16" s="2">
         <f t="shared" si="4"/>
-        <v>25403.200000000001</v>
+        <v>27528</v>
       </c>
       <c r="W16" s="1">
         <f>U16+MAX(E16*12-801,0)</f>
-        <v>28814.2</v>
+        <v>30939</v>
       </c>
       <c r="X16" s="1">
-        <f t="shared" si="6"/>
-        <v>25802.2</v>
+        <f t="shared" si="7"/>
+        <v>27927</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="7"/>
-        <v>5320.7999999999993</v>
+        <f t="shared" si="5"/>
+        <v>3196</v>
       </c>
       <c r="AA16">
         <f>(12*D16+(12*C16 - 920)*(C16&gt;450))</f>
@@ -2035,11 +2035,11 @@
         <v>0</v>
       </c>
       <c r="X17" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA17">
@@ -2118,23 +2118,23 @@
       </c>
       <c r="U18" s="2">
         <f>MAX(AA18-Z18-36-1308,0)</f>
-        <v>29151.8</v>
+        <v>29935</v>
       </c>
       <c r="V18" s="2">
         <f t="shared" si="4"/>
-        <v>26247.8</v>
+        <v>27031</v>
       </c>
       <c r="W18" s="1">
         <f>U18+MAX(E18*12-1370-51,0)</f>
-        <v>39730.800000000003</v>
+        <v>40514</v>
       </c>
       <c r="X18" s="1">
-        <f t="shared" si="6"/>
-        <v>36826.800000000003</v>
+        <f t="shared" si="7"/>
+        <v>37610</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="7"/>
-        <v>3163.2</v>
+        <f t="shared" si="5"/>
+        <v>2380</v>
       </c>
       <c r="AA18">
         <f>(12*D18+((12*C18)-920)*(C18&gt;450)+MAX((12*E18)-51-1370,0))</f>
@@ -2223,11 +2223,11 @@
         <v>0</v>
       </c>
       <c r="X19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA19">
@@ -2306,23 +2306,23 @@
       </c>
       <c r="U20" s="2">
         <f t="shared" ref="U20:U21" si="16">MAX(AA20-Z20-36,0)</f>
-        <v>18552.8</v>
+        <v>19336</v>
       </c>
       <c r="V20" s="2">
         <f t="shared" si="4"/>
-        <v>18552.8</v>
+        <v>19336</v>
       </c>
       <c r="W20" s="1">
         <f>U20+MAX(E20*12-801,0)</f>
-        <v>18552.8</v>
+        <v>19336</v>
       </c>
       <c r="X20" s="1">
-        <f t="shared" si="6"/>
-        <v>18552.8</v>
+        <f t="shared" si="7"/>
+        <v>19336</v>
       </c>
       <c r="Z20">
-        <f t="shared" si="7"/>
-        <v>4411.2</v>
+        <f t="shared" si="5"/>
+        <v>3628</v>
       </c>
       <c r="AA20">
         <f t="shared" si="15"/>
@@ -2411,11 +2411,11 @@
         <v>8758.4</v>
       </c>
       <c r="X21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8758.4</v>
       </c>
       <c r="Z21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>2205.6</v>
       </c>
       <c r="AA21">
@@ -2494,23 +2494,23 @@
       </c>
       <c r="U22" s="2">
         <f>0.5*(AA22+AA23-(Z22+Z23)-2*36)</f>
-        <v>23450</v>
+        <v>24904</v>
       </c>
       <c r="V22" s="2">
         <f t="shared" si="4"/>
-        <v>16022</v>
+        <v>17476</v>
       </c>
       <c r="W22" s="1">
         <f>U22+MAX(0.5*(E22*12-(2*801)),0)</f>
-        <v>23849</v>
+        <v>25303</v>
       </c>
       <c r="X22" s="1">
-        <f t="shared" si="6"/>
-        <v>16421</v>
+        <f t="shared" si="7"/>
+        <v>17875</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="7"/>
-        <v>6616.7999999999993</v>
+        <f t="shared" si="5"/>
+        <v>4492</v>
       </c>
       <c r="AA22">
         <f t="shared" si="15"/>
@@ -2589,23 +2589,23 @@
       </c>
       <c r="U23" s="2">
         <f>0.5*(AA22+AA23-(Z22+Z23)-2*36)</f>
-        <v>23450</v>
+        <v>24904</v>
       </c>
       <c r="V23" s="2">
         <f t="shared" si="4"/>
-        <v>16022</v>
+        <v>17476</v>
       </c>
       <c r="W23" s="1">
         <f>U22+MAX(0.5*(E22*12-(2*801)),0)</f>
-        <v>23849</v>
+        <v>25303</v>
       </c>
       <c r="X23" s="1">
-        <f t="shared" si="6"/>
-        <v>16421</v>
+        <f t="shared" si="7"/>
+        <v>17875</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="7"/>
-        <v>4411.2</v>
+        <f t="shared" si="5"/>
+        <v>3628</v>
       </c>
       <c r="AA23">
         <f t="shared" si="15"/>
@@ -2694,11 +2694,11 @@
         <v>0</v>
       </c>
       <c r="X24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA24">
@@ -2787,11 +2787,11 @@
         <v>0</v>
       </c>
       <c r="X25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA25">

</xml_diff>

<commit_message>
ALG test created. test no longer has its own param file. ui() is now doing the right thing. tarif() and soli_formula() are moved.
Former-commit-id: d5cd26d3d5a04a72fd413cce7024f904fc95343f
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_zve.xlsx
+++ b/tests/test_data/test_dfs_zve.xlsx
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD9" sqref="AD9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>